<commit_message>
sending updated code to Bitbucket
</commit_message>
<xml_diff>
--- a/TestData/PartyLite_Smokes_Data.xlsx
+++ b/TestData/PartyLite_Smokes_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\PartyLiteAn (1)\PartyLiteAn\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8491792C-C3E1-4D5F-B1E8-B629AB544702}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AC9B63-7489-469C-974D-C30927E61A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3036" yWindow="3036" windowWidth="17280" windowHeight="8964" firstSheet="48" activeTab="49" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="51" activeTab="55" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddGuestDetails_PL" sheetId="17" r:id="rId1"/>
@@ -20,80 +20,86 @@
     <sheet name="GuestOrderUSES_PL" sheetId="67" r:id="rId5"/>
     <sheet name="OEUS_PL" sheetId="68" r:id="rId6"/>
     <sheet name="OECA_PL" sheetId="69" r:id="rId7"/>
-    <sheet name="OEAU_PL" sheetId="82" r:id="rId8"/>
-    <sheet name="OEUK_PL" sheetId="83" r:id="rId9"/>
-    <sheet name="FYSPTUS_PL" sheetId="65" r:id="rId10"/>
-    <sheet name="Promotions_Coupon_PL" sheetId="19" r:id="rId11"/>
-    <sheet name="Cons_Send_Invitation_PL" sheetId="20" r:id="rId12"/>
-    <sheet name="Cons_RandomSend_PL" sheetId="50" r:id="rId13"/>
-    <sheet name="Collective_ConsAsHost_HA_PL" sheetId="25" r:id="rId14"/>
-    <sheet name="Facebook_ConsAsHost_HA_PL" sheetId="28" r:id="rId15"/>
-    <sheet name="Facebook_ConsAsHost_PA_PL" sheetId="29" r:id="rId16"/>
-    <sheet name="Facebook_ConsAsHost_NA_PL" sheetId="30" r:id="rId17"/>
-    <sheet name="FacebookParty_NH_PL" sheetId="31" r:id="rId18"/>
-    <sheet name="Facebook_PrevHost_HA_PL" sheetId="32" r:id="rId19"/>
-    <sheet name="Facebook_PrevHost_PA_PL" sheetId="33" r:id="rId20"/>
-    <sheet name="Facebook_PrevHost_NA_PL" sheetId="34" r:id="rId21"/>
-    <sheet name="PartyContactCreationDetails_PL" sheetId="16" r:id="rId22"/>
-    <sheet name="NCO_PL" sheetId="54" r:id="rId23"/>
-    <sheet name="ClassicPTUS_PL" sheetId="63" r:id="rId24"/>
-    <sheet name="Login_HostUser_PL" sheetId="36" r:id="rId25"/>
-    <sheet name="Nanosite_Guest_Check_PL" sheetId="37" r:id="rId26"/>
-    <sheet name="CreateAccount_NewUser_PL" sheetId="2" r:id="rId27"/>
-    <sheet name="Login_ExistingUser_PL" sheetId="1" r:id="rId28"/>
-    <sheet name="Login_ConsultantUser_PL" sheetId="5" r:id="rId29"/>
-    <sheet name="PartyCreationPrevHost_NA_PL" sheetId="13" r:id="rId30"/>
-    <sheet name="GuestOrder_PL" sheetId="14" r:id="rId31"/>
-    <sheet name="ProductSearch_PL" sheetId="80" r:id="rId32"/>
-    <sheet name="VirtualSearch_PL" sheetId="81" r:id="rId33"/>
-    <sheet name="DiscountDetail_PL" sheetId="79" r:id="rId34"/>
-    <sheet name="OrderLineType_PL" sheetId="76" r:id="rId35"/>
-    <sheet name="LineType_Coupon_US_PL" sheetId="77" r:id="rId36"/>
-    <sheet name="LineType_Coupon_CA_PL" sheetId="78" r:id="rId37"/>
-    <sheet name="CreateAccount_Address_PL" sheetId="52" r:id="rId38"/>
-    <sheet name="Login_AdminUser_PL" sheetId="15" r:id="rId39"/>
-    <sheet name="Nanosite_Guest_Order_PL" sheetId="21" r:id="rId40"/>
-    <sheet name="Nanosite_Account_Order_PL" sheetId="51" r:id="rId41"/>
-    <sheet name="Virtual_Outside_PL" sheetId="70" r:id="rId42"/>
-    <sheet name="PartyCreationDetails_PL" sheetId="6" r:id="rId43"/>
-    <sheet name="PartyCreationPrevHost_PA_PL" sheetId="12" r:id="rId44"/>
-    <sheet name="PartyCreationPrevHost_HA_PL" sheetId="11" r:id="rId45"/>
-    <sheet name="PartyCreationConsAsHost_NA_PL" sheetId="10" r:id="rId46"/>
-    <sheet name="PartyCreationConsAsHost_PA_PL" sheetId="9" r:id="rId47"/>
-    <sheet name="PartyCreationConsAsHost_HA_PL" sheetId="8" r:id="rId48"/>
-    <sheet name="VirtualSubmit_PL" sheetId="38" r:id="rId49"/>
-    <sheet name="CustomerOrder_PL" sheetId="22" r:id="rId50"/>
-    <sheet name="MyAccount_Email_PL" sheetId="71" r:id="rId51"/>
-    <sheet name="GuestOrder_GC_PL" sheetId="23" r:id="rId52"/>
-    <sheet name="CategoryURL_PL" sheetId="49" r:id="rId53"/>
-    <sheet name="PaperOrderCreationDetails_PL" sheetId="7" r:id="rId54"/>
-    <sheet name="CollectivePT_PL" sheetId="39" r:id="rId55"/>
-    <sheet name="CollectivePT_FR_PL" sheetId="73" r:id="rId56"/>
-    <sheet name="ClassicPT_PL" sheetId="35" r:id="rId57"/>
-    <sheet name="ClassicPT_FR_PL" sheetId="72" r:id="rId58"/>
-    <sheet name="PO_DB1_PL" sheetId="55" r:id="rId59"/>
-    <sheet name="PO_DB2_PL" sheetId="56" r:id="rId60"/>
-    <sheet name="PO_DB3_PL" sheetId="57" r:id="rId61"/>
-    <sheet name="PO_DB4_PL" sheetId="58" r:id="rId62"/>
-    <sheet name="PO_DB5_PL" sheetId="59" r:id="rId63"/>
-    <sheet name="PO_DB6_PL" sheetId="60" r:id="rId64"/>
-    <sheet name="PO_DB7_PL" sheetId="61" r:id="rId65"/>
-    <sheet name="PO_DB8_PL" sheetId="62" r:id="rId66"/>
-    <sheet name="FYSPT_PL" sheetId="40" r:id="rId67"/>
-    <sheet name="FYSPT_FR_PL" sheetId="74" r:id="rId68"/>
-    <sheet name="ClassicPTRC_PL" sheetId="41" r:id="rId69"/>
-    <sheet name="ClassicPT_SC_PL" sheetId="42" r:id="rId70"/>
-    <sheet name="CollectivePT_SC_PL" sheetId="43" r:id="rId71"/>
-    <sheet name="FYSPT_SC_PL" sheetId="44" r:id="rId72"/>
-    <sheet name="ClassicPT_SH_PL" sheetId="45" r:id="rId73"/>
-    <sheet name="CollectivePT_SH_PL" sheetId="46" r:id="rId74"/>
-    <sheet name="FYSPT_SH_PL" sheetId="47" r:id="rId75"/>
-    <sheet name="ClassicPTCA_PL" sheetId="64" r:id="rId76"/>
-    <sheet name="FYSPTCA_PL" sheetId="66" r:id="rId77"/>
-    <sheet name="ShareParty_PL" sheetId="48" r:id="rId78"/>
-    <sheet name="PartyContactCreationNano_PL" sheetId="24" r:id="rId79"/>
-    <sheet name="PreventDupeAcctCreation_PL" sheetId="3" r:id="rId80"/>
-    <sheet name="SearchConsultant_PL" sheetId="4" r:id="rId81"/>
+    <sheet name="OEFR_PL" sheetId="85" r:id="rId8"/>
+    <sheet name="OEAU_PL" sheetId="82" r:id="rId9"/>
+    <sheet name="OEUK_PL" sheetId="83" r:id="rId10"/>
+    <sheet name="FYSPTUS_PL" sheetId="65" r:id="rId11"/>
+    <sheet name="Promotions_Coupon_PL" sheetId="19" r:id="rId12"/>
+    <sheet name="Cons_Send_Invitation_PL" sheetId="20" r:id="rId13"/>
+    <sheet name="Cons_RandomSend_PL" sheetId="50" r:id="rId14"/>
+    <sheet name="Collective_ConsAsHost_HA_PL" sheetId="25" r:id="rId15"/>
+    <sheet name="Facebook_ConsAsHost_HA_PL" sheetId="28" r:id="rId16"/>
+    <sheet name="Facebook_ConsAsHost_PA_PL" sheetId="29" r:id="rId17"/>
+    <sheet name="Facebook_ConsAsHost_NA_PL" sheetId="30" r:id="rId18"/>
+    <sheet name="FacebookParty_NH_PL" sheetId="31" r:id="rId19"/>
+    <sheet name="Facebook_PrevHost_HA_PL" sheetId="32" r:id="rId20"/>
+    <sheet name="Facebook_PrevHost_PA_PL" sheetId="33" r:id="rId21"/>
+    <sheet name="Facebook_PrevHost_NA_PL" sheetId="34" r:id="rId22"/>
+    <sheet name="PartyContactCreationDetails_PL" sheetId="16" r:id="rId23"/>
+    <sheet name="NCO_PL" sheetId="54" r:id="rId24"/>
+    <sheet name="ClassicPTUS_PL" sheetId="63" r:id="rId25"/>
+    <sheet name="Login_HostUser_PL" sheetId="36" r:id="rId26"/>
+    <sheet name="Nanosite_Guest_Check_PL" sheetId="37" r:id="rId27"/>
+    <sheet name="CreateAccount_NewUser_PL" sheetId="2" r:id="rId28"/>
+    <sheet name="Login_ExistingUser_PL" sheetId="1" r:id="rId29"/>
+    <sheet name="Login_ConsultantUser_PL" sheetId="5" r:id="rId30"/>
+    <sheet name="PartyCreationPrevHost_NA_PL" sheetId="13" r:id="rId31"/>
+    <sheet name="GuestOrder_PL" sheetId="14" r:id="rId32"/>
+    <sheet name="ProductSearch_PL" sheetId="80" r:id="rId33"/>
+    <sheet name="VirtualSearch_PL" sheetId="81" r:id="rId34"/>
+    <sheet name="DiscountDetail_PL" sheetId="79" r:id="rId35"/>
+    <sheet name="OrderLineType_PL" sheetId="76" r:id="rId36"/>
+    <sheet name="LineType_Coupon_US_PL" sheetId="77" r:id="rId37"/>
+    <sheet name="LineType_Coupon_CA_PL" sheetId="78" r:id="rId38"/>
+    <sheet name="CreateAccount_Address_PL" sheetId="52" r:id="rId39"/>
+    <sheet name="Login_AdminUser_PL" sheetId="15" r:id="rId40"/>
+    <sheet name="Nanosite_Guest_Order_PL" sheetId="21" r:id="rId41"/>
+    <sheet name="Nanosite_Account_Order_PL" sheetId="51" r:id="rId42"/>
+    <sheet name="Virtual_Outside_PL" sheetId="70" r:id="rId43"/>
+    <sheet name="PartyCreationDetails_PL" sheetId="6" r:id="rId44"/>
+    <sheet name="PartyCreationPrevHost_PA_PL" sheetId="12" r:id="rId45"/>
+    <sheet name="PartyCreationPrevHost_HA_PL" sheetId="11" r:id="rId46"/>
+    <sheet name="PartyCreationConsAsHost_NA_PL" sheetId="10" r:id="rId47"/>
+    <sheet name="PartyCreationConsAsHost_PA_PL" sheetId="9" r:id="rId48"/>
+    <sheet name="PartyCreationConsAsHost_HA_PL" sheetId="8" r:id="rId49"/>
+    <sheet name="VirtualSubmit_PL" sheetId="38" r:id="rId50"/>
+    <sheet name="CustomerOrder_PL" sheetId="22" r:id="rId51"/>
+    <sheet name="Smoke_TestCase_2" sheetId="84" r:id="rId52"/>
+    <sheet name="Smoke_TestCase_3" sheetId="86" r:id="rId53"/>
+    <sheet name="Smoke_TestCase_6" sheetId="87" r:id="rId54"/>
+    <sheet name="Smoke_TestCase_7" sheetId="88" r:id="rId55"/>
+    <sheet name="Smoke_TestCase_8" sheetId="89" r:id="rId56"/>
+    <sheet name="MyAccount_Email_PL" sheetId="71" r:id="rId57"/>
+    <sheet name="GuestOrder_GC_PL" sheetId="23" r:id="rId58"/>
+    <sheet name="CategoryURL_PL" sheetId="49" r:id="rId59"/>
+    <sheet name="PaperOrderCreationDetails_PL" sheetId="7" r:id="rId60"/>
+    <sheet name="CollectivePT_PL" sheetId="39" r:id="rId61"/>
+    <sheet name="CollectivePT_FR_PL" sheetId="73" r:id="rId62"/>
+    <sheet name="ClassicPT_PL" sheetId="35" r:id="rId63"/>
+    <sheet name="ClassicPT_FR_PL" sheetId="72" r:id="rId64"/>
+    <sheet name="PO_DB1_PL" sheetId="55" r:id="rId65"/>
+    <sheet name="PO_DB2_PL" sheetId="56" r:id="rId66"/>
+    <sheet name="PO_DB3_PL" sheetId="57" r:id="rId67"/>
+    <sheet name="PO_DB4_PL" sheetId="58" r:id="rId68"/>
+    <sheet name="PO_DB5_PL" sheetId="59" r:id="rId69"/>
+    <sheet name="PO_DB6_PL" sheetId="60" r:id="rId70"/>
+    <sheet name="PO_DB7_PL" sheetId="61" r:id="rId71"/>
+    <sheet name="PO_DB8_PL" sheetId="62" r:id="rId72"/>
+    <sheet name="FYSPT_PL" sheetId="40" r:id="rId73"/>
+    <sheet name="FYSPT_FR_PL" sheetId="74" r:id="rId74"/>
+    <sheet name="ClassicPTRC_PL" sheetId="41" r:id="rId75"/>
+    <sheet name="ClassicPT_SC_PL" sheetId="42" r:id="rId76"/>
+    <sheet name="CollectivePT_SC_PL" sheetId="43" r:id="rId77"/>
+    <sheet name="FYSPT_SC_PL" sheetId="44" r:id="rId78"/>
+    <sheet name="ClassicPT_SH_PL" sheetId="45" r:id="rId79"/>
+    <sheet name="CollectivePT_SH_PL" sheetId="46" r:id="rId80"/>
+    <sheet name="FYSPT_SH_PL" sheetId="47" r:id="rId81"/>
+    <sheet name="ClassicPTCA_PL" sheetId="64" r:id="rId82"/>
+    <sheet name="FYSPTCA_PL" sheetId="66" r:id="rId83"/>
+    <sheet name="ShareParty_PL" sheetId="48" r:id="rId84"/>
+    <sheet name="PartyContactCreationNano_PL" sheetId="24" r:id="rId85"/>
+    <sheet name="PreventDupeAcctCreation_PL" sheetId="3" r:id="rId86"/>
+    <sheet name="SearchConsultant_PL" sheetId="4" r:id="rId87"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -105,7 +111,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3122" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3311" uniqueCount="392">
   <si>
     <t>Username</t>
   </si>
@@ -1167,6 +1173,120 @@
   </si>
   <si>
     <t>test1party@test.com</t>
+  </si>
+  <si>
+    <t>FS29</t>
+  </si>
+  <si>
+    <t>2240 Aimama Pl</t>
+  </si>
+  <si>
+    <t>96782-1335</t>
+  </si>
+  <si>
+    <t>Pearl City</t>
+  </si>
+  <si>
+    <t>Hawaii</t>
+  </si>
+  <si>
+    <t>1sqa@work!</t>
+  </si>
+  <si>
+    <t>test_smoke2109shashwat@mailinator.com</t>
+  </si>
+  <si>
+    <t>test_smoke2209shashwat@mailinator.com</t>
+  </si>
+  <si>
+    <t>Shashwat</t>
+  </si>
+  <si>
+    <t>9 Euclid St</t>
+  </si>
+  <si>
+    <t>Unionville</t>
+  </si>
+  <si>
+    <t>L3R 1P5</t>
+  </si>
+  <si>
+    <t>Ontario</t>
+  </si>
+  <si>
+    <t>Victoria</t>
+  </si>
+  <si>
+    <t>addressbill</t>
+  </si>
+  <si>
+    <t>citybill</t>
+  </si>
+  <si>
+    <t>statebill</t>
+  </si>
+  <si>
+    <t>zipbill</t>
+  </si>
+  <si>
+    <t>9 Eden Street</t>
+  </si>
+  <si>
+    <t>Gladstone</t>
+  </si>
+  <si>
+    <t>Queensland</t>
+  </si>
+  <si>
+    <t>test_smoke2209guest@mailinator.com</t>
+  </si>
+  <si>
+    <t>434 Dorcas St</t>
+  </si>
+  <si>
+    <t>South Melbourne</t>
+  </si>
+  <si>
+    <t>Allée de l'Orme Rond</t>
+  </si>
+  <si>
+    <t>Bailly-Romainvilliers</t>
+  </si>
+  <si>
+    <t>addressRC</t>
+  </si>
+  <si>
+    <t>cityRC</t>
+  </si>
+  <si>
+    <t>zipRC</t>
+  </si>
+  <si>
+    <t>9876787612</t>
+  </si>
+  <si>
+    <t>test_smoke2309guestpwsauto@mailinator.com</t>
+  </si>
+  <si>
+    <t>PayPal</t>
+  </si>
+  <si>
+    <t>Heidelberger Mühle</t>
+  </si>
+  <si>
+    <t>Groß Pankow</t>
+  </si>
+  <si>
+    <t>Prignitz</t>
+  </si>
+  <si>
+    <t>dedemagqa@mailinator.com</t>
+  </si>
+  <si>
+    <t>emailsubscribe</t>
+  </si>
+  <si>
+    <t>test_smoke0923@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -1334,7 +1454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1369,6 +1489,14 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1867,6 +1995,88 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>338</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -2056,7 +2266,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:F3"/>
   <sheetViews>
@@ -2131,7 +2341,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -2201,7 +2411,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -2277,7 +2487,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <dimension ref="A1:G2"/>
   <sheetViews>
@@ -2341,7 +2551,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2393,7 +2603,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -2445,7 +2655,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -2533,7 +2743,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -2634,65 +2844,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>131</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2333</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>220</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2816,6 +2967,65 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>131</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2333</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -2874,7 +3084,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
@@ -2969,7 +3179,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J2"/>
@@ -3058,7 +3268,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -3189,7 +3399,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -3380,7 +3590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3439,7 +3649,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -3467,7 +3677,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F2"/>
@@ -3532,7 +3742,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Q2"/>
@@ -3662,7 +3872,125 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:P2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="17.399999999999999">
+      <c r="A2" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="qacwscategory_guestorder@mailinator.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B2"/>
@@ -3698,125 +4026,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:P2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" t="s">
-        <v>215</v>
-      </c>
-      <c r="L1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="17.399999999999999">
-      <c r="A2" s="16" t="s">
-        <v>97</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>252</v>
-      </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="qacwscategory_guestorder@mailinator.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Q2"/>
@@ -3942,13 +4152,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:R2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:R3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -4076,7 +4286,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4107,7 +4317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
   <dimension ref="A1:E79"/>
   <sheetViews>
@@ -4941,7 +5151,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4973,7 +5183,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
@@ -5313,7 +5523,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
@@ -5674,7 +5884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
   <dimension ref="A1:R6"/>
   <sheetViews>
@@ -6028,7 +6238,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
   <dimension ref="A1:L11"/>
   <sheetViews>
@@ -6485,7 +6695,125 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>163</v>
+      </c>
+      <c r="B1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>62</v>
+      </c>
+      <c r="G1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" t="s">
+        <v>64</v>
+      </c>
+      <c r="I1" t="s">
+        <v>44</v>
+      </c>
+      <c r="J1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L1" t="s">
+        <v>46</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="17.399999999999999">
+      <c r="A2" s="16" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F2" t="s">
+        <v>283</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="L2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="qacwscategory_guestorder@mailinator.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:B2"/>
@@ -6521,125 +6849,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>163</v>
-      </c>
-      <c r="B1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
-      </c>
-      <c r="E1" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" t="s">
-        <v>62</v>
-      </c>
-      <c r="G1" t="s">
-        <v>63</v>
-      </c>
-      <c r="H1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" t="s">
-        <v>65</v>
-      </c>
-      <c r="K1" t="s">
-        <v>215</v>
-      </c>
-      <c r="L1" t="s">
-        <v>46</v>
-      </c>
-      <c r="M1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="17.399999999999999">
-      <c r="A2" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>282</v>
-      </c>
-      <c r="C2" t="s">
-        <v>66</v>
-      </c>
-      <c r="D2" t="s">
-        <v>67</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="F2" t="s">
-        <v>283</v>
-      </c>
-      <c r="G2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="qacwscategory_guestorder@mailinator.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
   <dimension ref="A1:O2"/>
   <sheetViews>
@@ -6748,7 +6958,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -6869,7 +7079,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -6966,7 +7176,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:S2"/>
@@ -7107,7 +7317,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:F2"/>
@@ -7170,7 +7380,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:F2"/>
@@ -7230,7 +7440,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:P2"/>
@@ -7349,7 +7559,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:E2"/>
@@ -7402,7 +7612,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:E2"/>
@@ -7450,76 +7660,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-2F00-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
-  <dimension ref="A1:H2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:8">
-      <c r="A1" t="s">
-        <v>116</v>
-      </c>
-      <c r="B1" t="s">
-        <v>117</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>45</v>
-      </c>
-      <c r="E1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" t="s">
-        <v>49</v>
-      </c>
-      <c r="H1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="1" t="s">
-        <v>200</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>125</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>285</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-3000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -7651,11 +7791,81 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
+  <dimension ref="A1:H2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="A1" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G1" t="s">
+        <v>49</v>
+      </c>
+      <c r="H1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>285</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-3000-000000000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
   <dimension ref="A1:Q6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -7789,7 +7999,733 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00557CE2-344E-4748-8050-502ACD386C65}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17.399999999999999">
+      <c r="A2" s="1" t="s">
+        <v>360</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="E2" s="16">
+        <v>1</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>355</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>356</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>357</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>358</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" s="4">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{F0A9B555-A9E5-4569-8C63-F3EB03DD41FA}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{8F42B2BA-72E7-4561-A341-C3A2E2747D66}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF99577-3E21-4F91-8A0E-F977C7E7598B}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="3" max="3" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.69921875" customWidth="1"/>
+    <col min="6" max="6" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17.399999999999999">
+      <c r="A2" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>366</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" s="4">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{209DDE12-9F8E-43EB-ADC3-96C4571EC58A}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377BF7CB-F633-49F4-8D49-EB8446EAC16C}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:U2"/>
+  <sheetViews>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="D1" sqref="A1:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="2" max="2" width="4.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.296875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.8984375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" t="s">
+        <v>215</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+      <c r="R1" t="s">
+        <v>368</v>
+      </c>
+      <c r="S1" t="s">
+        <v>369</v>
+      </c>
+      <c r="T1" t="s">
+        <v>370</v>
+      </c>
+      <c r="U1" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="17.399999999999999">
+      <c r="A2" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="B2" s="16">
+        <v>1</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>375</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="G2" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="2">
+        <v>3205</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>377</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" s="4">
+        <v>23</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="R2" t="s">
+        <v>372</v>
+      </c>
+      <c r="S2" t="s">
+        <v>373</v>
+      </c>
+      <c r="T2" t="s">
+        <v>374</v>
+      </c>
+      <c r="U2">
+        <v>4680</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{807A3D09-D1F7-43E4-8612-AABB53C9F8DD}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E84195DF-01B2-4D45-8E2B-90A4FB63FF02}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="8.796875" style="33"/>
+    <col min="2" max="2" width="4.19921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.69921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.59765625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.796875" style="33"/>
+    <col min="9" max="9" width="7.296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.296875" style="33" customWidth="1"/>
+    <col min="12" max="12" width="18.296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>62</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>63</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>380</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>381</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>382</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" s="33" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" s="33" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" s="33" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="17.399999999999999">
+      <c r="A2" s="34" t="s">
+        <v>354</v>
+      </c>
+      <c r="B2" s="35">
+        <v>1</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>384</v>
+      </c>
+      <c r="D2" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>378</v>
+      </c>
+      <c r="G2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="H2" s="33" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" s="32">
+        <v>77700</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>379</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>383</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>378</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>379</v>
+      </c>
+      <c r="N2" s="32">
+        <v>77700</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>385</v>
+      </c>
+      <c r="P2" s="38" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="R2" s="39">
+        <v>23</v>
+      </c>
+      <c r="S2" s="39" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{318A39AA-72BA-4A66-A3C8-5DCE254FC2E2}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622CFA83-E905-4467-BCFD-8E7E2CF53AA9}">
+  <dimension ref="A1:R2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.3984375" customWidth="1"/>
+    <col min="4" max="4" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>390</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F1" t="s">
+        <v>221</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" ht="17.399999999999999">
+      <c r="A2" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>391</v>
+      </c>
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="F2" s="16">
+        <v>1</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="2">
+        <v>16928</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>387</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q2" s="4">
+        <v>23</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{83A341BD-A415-4EC1-9C7D-53D27E82D078}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{A0B128BF-5C69-492F-9E25-60EC8B6D8510}"/>
+    <hyperlink ref="C2" r:id="rId3" xr:uid="{4DCE5C32-E792-4E94-959E-DB85BFA4F127}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -7842,7 +8778,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
@@ -8395,7 +9331,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
@@ -8475,7 +9411,86 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AB2"/>
@@ -8675,7 +9690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -8794,7 +9809,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -8913,7 +9928,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -9104,7 +10119,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -9295,7 +10310,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -9486,86 +10501,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -9756,7 +10692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -9947,7 +10883,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10138,7 +11074,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10329,7 +11265,86 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.8">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10520,7 +11535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10711,7 +11726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10902,7 +11917,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11093,7 +12108,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11284,7 +12299,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11476,86 +12491,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.8">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>261</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11746,7 +12682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -11865,7 +12801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12056,7 +12992,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12247,7 +13183,91 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCF2C1E-628B-4BC7-AE6E-3B1E5B8F517C}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.09765625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.8">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -12366,7 +13386,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12558,7 +13578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12749,7 +13769,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4C00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12940,7 +13960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4D00-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -13046,7 +14066,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4E00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -13098,89 +14118,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <cols>
-    <col min="5" max="5" width="11.19921875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4F00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:F2"/>
@@ -13243,7 +14181,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5000-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:D2"/>
@@ -13289,16 +14227,16 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
   <cols>
-    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.19921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -13338,19 +14276,19 @@
         <v>23</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>337</v>
+        <v>330</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>338</v>
+        <v>328</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>331</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="G2" s="6" t="s">
         <v>214</v>

</xml_diff>

<commit_message>
new changes after smoke test cases are ready
</commit_message>
<xml_diff>
--- a/TestData/PartyLite_Smokes_Data.xlsx
+++ b/TestData/PartyLite_Smokes_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\PartyLiteAn (1)\PartyLiteAn\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89AC9B63-7489-469C-974D-C30927E61A8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F9B829-89FE-4575-96AC-E37FE6CC6A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="51" activeTab="55" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="54" activeTab="56" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddGuestDetails_PL" sheetId="17" r:id="rId1"/>
@@ -69,37 +69,40 @@
     <sheet name="Smoke_TestCase_6" sheetId="87" r:id="rId54"/>
     <sheet name="Smoke_TestCase_7" sheetId="88" r:id="rId55"/>
     <sheet name="Smoke_TestCase_8" sheetId="89" r:id="rId56"/>
-    <sheet name="MyAccount_Email_PL" sheetId="71" r:id="rId57"/>
-    <sheet name="GuestOrder_GC_PL" sheetId="23" r:id="rId58"/>
-    <sheet name="CategoryURL_PL" sheetId="49" r:id="rId59"/>
-    <sheet name="PaperOrderCreationDetails_PL" sheetId="7" r:id="rId60"/>
-    <sheet name="CollectivePT_PL" sheetId="39" r:id="rId61"/>
-    <sheet name="CollectivePT_FR_PL" sheetId="73" r:id="rId62"/>
-    <sheet name="ClassicPT_PL" sheetId="35" r:id="rId63"/>
-    <sheet name="ClassicPT_FR_PL" sheetId="72" r:id="rId64"/>
-    <sheet name="PO_DB1_PL" sheetId="55" r:id="rId65"/>
-    <sheet name="PO_DB2_PL" sheetId="56" r:id="rId66"/>
-    <sheet name="PO_DB3_PL" sheetId="57" r:id="rId67"/>
-    <sheet name="PO_DB4_PL" sheetId="58" r:id="rId68"/>
-    <sheet name="PO_DB5_PL" sheetId="59" r:id="rId69"/>
-    <sheet name="PO_DB6_PL" sheetId="60" r:id="rId70"/>
-    <sheet name="PO_DB7_PL" sheetId="61" r:id="rId71"/>
-    <sheet name="PO_DB8_PL" sheetId="62" r:id="rId72"/>
-    <sheet name="FYSPT_PL" sheetId="40" r:id="rId73"/>
-    <sheet name="FYSPT_FR_PL" sheetId="74" r:id="rId74"/>
-    <sheet name="ClassicPTRC_PL" sheetId="41" r:id="rId75"/>
-    <sheet name="ClassicPT_SC_PL" sheetId="42" r:id="rId76"/>
-    <sheet name="CollectivePT_SC_PL" sheetId="43" r:id="rId77"/>
-    <sheet name="FYSPT_SC_PL" sheetId="44" r:id="rId78"/>
-    <sheet name="ClassicPT_SH_PL" sheetId="45" r:id="rId79"/>
-    <sheet name="CollectivePT_SH_PL" sheetId="46" r:id="rId80"/>
-    <sheet name="FYSPT_SH_PL" sheetId="47" r:id="rId81"/>
-    <sheet name="ClassicPTCA_PL" sheetId="64" r:id="rId82"/>
-    <sheet name="FYSPTCA_PL" sheetId="66" r:id="rId83"/>
-    <sheet name="ShareParty_PL" sheetId="48" r:id="rId84"/>
-    <sheet name="PartyContactCreationNano_PL" sheetId="24" r:id="rId85"/>
-    <sheet name="PreventDupeAcctCreation_PL" sheetId="3" r:id="rId86"/>
-    <sheet name="SearchConsultant_PL" sheetId="4" r:id="rId87"/>
+    <sheet name="Smoke_TestCase_10" sheetId="90" r:id="rId57"/>
+    <sheet name="Smoke_TestCase_11" sheetId="91" r:id="rId58"/>
+    <sheet name="Smoke_TestCase_12" sheetId="92" r:id="rId59"/>
+    <sheet name="MyAccount_Email_PL" sheetId="71" r:id="rId60"/>
+    <sheet name="GuestOrder_GC_PL" sheetId="23" r:id="rId61"/>
+    <sheet name="CategoryURL_PL" sheetId="49" r:id="rId62"/>
+    <sheet name="PaperOrderCreationDetails_PL" sheetId="7" r:id="rId63"/>
+    <sheet name="CollectivePT_PL" sheetId="39" r:id="rId64"/>
+    <sheet name="CollectivePT_FR_PL" sheetId="73" r:id="rId65"/>
+    <sheet name="ClassicPT_PL" sheetId="35" r:id="rId66"/>
+    <sheet name="ClassicPT_FR_PL" sheetId="72" r:id="rId67"/>
+    <sheet name="PO_DB1_PL" sheetId="55" r:id="rId68"/>
+    <sheet name="PO_DB2_PL" sheetId="56" r:id="rId69"/>
+    <sheet name="PO_DB3_PL" sheetId="57" r:id="rId70"/>
+    <sheet name="PO_DB4_PL" sheetId="58" r:id="rId71"/>
+    <sheet name="PO_DB5_PL" sheetId="59" r:id="rId72"/>
+    <sheet name="PO_DB6_PL" sheetId="60" r:id="rId73"/>
+    <sheet name="PO_DB7_PL" sheetId="61" r:id="rId74"/>
+    <sheet name="PO_DB8_PL" sheetId="62" r:id="rId75"/>
+    <sheet name="FYSPT_PL" sheetId="40" r:id="rId76"/>
+    <sheet name="FYSPT_FR_PL" sheetId="74" r:id="rId77"/>
+    <sheet name="ClassicPTRC_PL" sheetId="41" r:id="rId78"/>
+    <sheet name="ClassicPT_SC_PL" sheetId="42" r:id="rId79"/>
+    <sheet name="CollectivePT_SC_PL" sheetId="43" r:id="rId80"/>
+    <sheet name="FYSPT_SC_PL" sheetId="44" r:id="rId81"/>
+    <sheet name="ClassicPT_SH_PL" sheetId="45" r:id="rId82"/>
+    <sheet name="CollectivePT_SH_PL" sheetId="46" r:id="rId83"/>
+    <sheet name="FYSPT_SH_PL" sheetId="47" r:id="rId84"/>
+    <sheet name="ClassicPTCA_PL" sheetId="64" r:id="rId85"/>
+    <sheet name="FYSPTCA_PL" sheetId="66" r:id="rId86"/>
+    <sheet name="ShareParty_PL" sheetId="48" r:id="rId87"/>
+    <sheet name="PartyContactCreationNano_PL" sheetId="24" r:id="rId88"/>
+    <sheet name="PreventDupeAcctCreation_PL" sheetId="3" r:id="rId89"/>
+    <sheet name="SearchConsultant_PL" sheetId="4" r:id="rId90"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -111,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3311" uniqueCount="392">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3400" uniqueCount="414">
   <si>
     <t>Username</t>
   </si>
@@ -1286,7 +1289,73 @@
     <t>emailsubscribe</t>
   </si>
   <si>
-    <t>test_smoke0923@mailinator.com</t>
+    <t>subscribername</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39 Broughton </t>
+  </si>
+  <si>
+    <t>Glasgow</t>
+  </si>
+  <si>
+    <t>G75 0JU</t>
+  </si>
+  <si>
+    <t>Mishra</t>
+  </si>
+  <si>
+    <t>confemail</t>
+  </si>
+  <si>
+    <t>SKU1</t>
+  </si>
+  <si>
+    <t>P93141</t>
+  </si>
+  <si>
+    <t>SKU2</t>
+  </si>
+  <si>
+    <t>SKU3</t>
+  </si>
+  <si>
+    <t>V06199</t>
+  </si>
+  <si>
+    <t>Mainhartsdorf 1</t>
+  </si>
+  <si>
+    <t>OBERWÖLZ</t>
+  </si>
+  <si>
+    <t>test_smoke1001shashwat@mailinator.com</t>
+  </si>
+  <si>
+    <t>079 294 04 91</t>
+  </si>
+  <si>
+    <t>GB109_091LW6K</t>
+  </si>
+  <si>
+    <t>GC-15</t>
+  </si>
+  <si>
+    <t>chsqanew02@mailinator.com</t>
+  </si>
+  <si>
+    <t>Konkordiastr. 28</t>
+  </si>
+  <si>
+    <t>St. Gallen</t>
+  </si>
+  <si>
+    <t>chsqanew</t>
+  </si>
+  <si>
+    <t>uksqanew</t>
+  </si>
+  <si>
+    <t>test_smoke</t>
   </si>
 </sst>
 </file>
@@ -1454,7 +1523,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1497,6 +1566,9 @@
     <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -3683,7 +3755,7 @@
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F7" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
@@ -8007,7 +8079,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -8142,7 +8214,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -8438,7 +8510,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -8587,23 +8659,27 @@
 
 <file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622CFA83-E905-4467-BCFD-8E7E2CF53AA9}">
-  <dimension ref="A1:R2"/>
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="25.59765625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.3984375" customWidth="1"/>
-    <col min="4" max="4" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.3984375" customWidth="1"/>
+    <col min="5" max="5" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -8614,52 +8690,55 @@
         <v>390</v>
       </c>
       <c r="D1" t="s">
+        <v>391</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>221</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>61</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>62</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>63</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>215</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>65</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>46</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>47</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>49</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.399999999999999">
+    <row r="2" spans="1:19" ht="17.399999999999999">
       <c r="A2" s="1" t="s">
         <v>389</v>
       </c>
@@ -8667,51 +8746,54 @@
         <v>359</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>391</v>
+        <v>413</v>
       </c>
       <c r="D2" t="s">
+        <v>362</v>
+      </c>
+      <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>354</v>
       </c>
-      <c r="F2" s="16">
+      <c r="G2" s="16">
         <v>1</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>386</v>
-      </c>
-      <c r="H2" t="s">
-        <v>69</v>
       </c>
       <c r="I2" t="s">
         <v>69</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="2">
         <v>16928</v>
       </c>
-      <c r="K2" s="2" t="s">
+      <c r="L2" s="2" t="s">
         <v>387</v>
       </c>
-      <c r="L2" s="2" t="s">
+      <c r="M2" s="2" t="s">
         <v>388</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="N2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="O2" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="O2" s="6" t="s">
+      <c r="P2" s="6" t="s">
         <v>118</v>
       </c>
-      <c r="P2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" s="4">
+      <c r="R2" s="4">
         <v>23</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>51</v>
       </c>
     </row>
@@ -8719,694 +8801,398 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" xr:uid="{83A341BD-A415-4EC1-9C7D-53D27E82D078}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{A0B128BF-5C69-492F-9E25-60EC8B6D8510}"/>
-    <hyperlink ref="C2" r:id="rId3" xr:uid="{4DCE5C32-E792-4E94-959E-DB85BFA4F127}"/>
+    <hyperlink ref="C2" r:id="rId3" display="test_smoke0410@mailinator.com" xr:uid="{4DCE5C32-E792-4E94-959E-DB85BFA4F127}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
-  <dimension ref="A1:C3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9962DFF2-70D3-42DF-A705-EB69D22B5F41}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="2" width="8.796875" style="33"/>
+    <col min="3" max="4" width="9.296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.19921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.796875" style="33"/>
+    <col min="9" max="9" width="15.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.796875" style="33"/>
+    <col min="13" max="13" width="11.8984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.8984375" style="33" customWidth="1"/>
+    <col min="15" max="16384" width="8.796875" style="33"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15">
+      <c r="A1" s="33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D1" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="C1" t="s">
+      <c r="F1" s="33" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="1" t="s">
-        <v>264</v>
-      </c>
-      <c r="B2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="G1" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15" ht="17.399999999999999">
+      <c r="A2" s="33" t="s">
+        <v>362</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>395</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>412</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>412</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>359</v>
+      </c>
+      <c r="F2" s="33" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>4</v>
+      <c r="G2" s="34" t="s">
+        <v>354</v>
+      </c>
+      <c r="H2" s="35">
+        <v>1</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>392</v>
+      </c>
+      <c r="J2" s="32" t="s">
+        <v>394</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>393</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>388</v>
+      </c>
+      <c r="M2" s="32">
+        <v>1923123457</v>
+      </c>
+      <c r="N2" s="33" t="s">
+        <v>406</v>
+      </c>
+      <c r="O2" s="37" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-3200-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" display="testconsultant3@mailinator.com" xr:uid="{00000000-0004-0000-3200-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-3200-000002000000}"/>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{83C30567-2619-416A-8A3B-3616C36A4346}"/>
+    <hyperlink ref="C2" r:id="rId2" display="uksqanew10@mailinator.com" xr:uid="{1B909638-F0A6-424A-A3B0-75B23D4BBC00}"/>
+    <hyperlink ref="D2" r:id="rId3" display="uksqanew10@mailinator.com" xr:uid="{DCFC5EAD-59D0-4AF8-B14D-9C3562C8FA05}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
-  <dimension ref="A1:Q10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABC2C4D-D525-4D71-9D7D-8F9EC67442AC}">
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="1" width="11" style="30"/>
+    <col min="1" max="3" width="8.796875" style="33"/>
+    <col min="4" max="4" width="4.19921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.69921875" style="33" customWidth="1"/>
+    <col min="6" max="6" width="18.69921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.59765625" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.796875" style="33"/>
+    <col min="11" max="11" width="11.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.796875" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="30" t="s">
-        <v>60</v>
-      </c>
-      <c r="B1" t="s">
-        <v>121</v>
-      </c>
-      <c r="C1" t="s">
-        <v>122</v>
-      </c>
-      <c r="D1" t="s">
+    <row r="1" spans="1:18">
+      <c r="A1" s="33" t="s">
+        <v>397</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>400</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="F1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="H1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="H1" t="s">
+      <c r="J1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="I1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="K1" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" s="33" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.399999999999999">
-      <c r="A2" s="31" t="s">
-        <v>285</v>
-      </c>
-      <c r="B2" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E2" t="s">
-        <v>66</v>
-      </c>
-      <c r="F2" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" t="s">
+    <row r="2" spans="1:18" ht="17.399999999999999">
+      <c r="A2" s="34" t="s">
+        <v>398</v>
+      </c>
+      <c r="B2" s="34" t="s">
+        <v>401</v>
+      </c>
+      <c r="C2" s="34" t="s">
+        <v>289</v>
+      </c>
+      <c r="D2" s="35">
+        <v>2</v>
+      </c>
+      <c r="E2" s="32" t="s">
+        <v>351</v>
+      </c>
+      <c r="F2" s="36" t="s">
+        <v>404</v>
+      </c>
+      <c r="G2" s="32" t="s">
+        <v>362</v>
+      </c>
+      <c r="H2" s="32" t="s">
+        <v>84</v>
+      </c>
+      <c r="I2" s="32" t="s">
+        <v>402</v>
+      </c>
+      <c r="J2" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="I2" t="s">
-        <v>69</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M2" s="11" t="s">
+      <c r="K2" s="40">
+        <v>8832</v>
+      </c>
+      <c r="L2" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="N2" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="O2" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="P2" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" ht="17.399999999999999">
-      <c r="A3" s="31" t="s">
-        <v>342</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>173</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E3" t="s">
-        <v>66</v>
-      </c>
-      <c r="F3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" t="s">
-        <v>69</v>
-      </c>
-      <c r="J3" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M3" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="N3" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="O3" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="P3" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q3" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" ht="17.399999999999999">
-      <c r="A4" s="31" t="s">
-        <v>343</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>177</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E4" t="s">
-        <v>66</v>
-      </c>
-      <c r="F4" t="s">
-        <v>67</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" t="s">
-        <v>69</v>
-      </c>
-      <c r="I4" t="s">
-        <v>69</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K4" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L4" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M4" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="O4" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="P4" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q4" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" ht="17.399999999999999">
-      <c r="A5" s="31" t="s">
-        <v>344</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="C5" t="s">
-        <v>174</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E5" t="s">
-        <v>66</v>
-      </c>
-      <c r="F5" t="s">
-        <v>67</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H5" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" t="s">
-        <v>69</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M5" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="N5" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="O5" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="P5" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q5" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" ht="17.399999999999999">
-      <c r="A6" s="31" t="s">
-        <v>345</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>168</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E6" t="s">
-        <v>66</v>
-      </c>
-      <c r="F6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H6" t="s">
-        <v>69</v>
-      </c>
-      <c r="I6" t="s">
-        <v>69</v>
-      </c>
-      <c r="J6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L6" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M6" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="N6" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="O6" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="P6" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q6" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" ht="17.399999999999999">
-      <c r="A7" s="31" t="s">
-        <v>346</v>
-      </c>
-      <c r="B7" t="s">
-        <v>169</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E7" t="s">
-        <v>66</v>
-      </c>
-      <c r="F7" t="s">
-        <v>67</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H7" t="s">
-        <v>69</v>
-      </c>
-      <c r="I7" t="s">
-        <v>69</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K7" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M7" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="N7" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="O7" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="P7" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q7" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" ht="17.399999999999999">
-      <c r="A8" s="31" t="s">
-        <v>347</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>170</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>178</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H8" t="s">
-        <v>69</v>
-      </c>
-      <c r="I8" t="s">
-        <v>69</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K8" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L8" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M8" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="N8" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="O8" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="P8" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q8" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" ht="17.399999999999999">
-      <c r="A9" s="31" t="s">
-        <v>348</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>171</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" t="s">
-        <v>69</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K9" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L9" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M9" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="N9" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="O9" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="P9" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q9" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" ht="17.399999999999999">
-      <c r="A10" s="31" t="s">
-        <v>349</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>172</v>
-      </c>
-      <c r="C10" s="4" t="s">
-        <v>179</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="E10" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" t="s">
-        <v>67</v>
-      </c>
-      <c r="G10" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H10" t="s">
-        <v>69</v>
-      </c>
-      <c r="I10" t="s">
-        <v>69</v>
-      </c>
-      <c r="J10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="L10" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="M10" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="N10" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="O10" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="P10" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="Q10" s="4" t="s">
+      <c r="Q2" s="39">
+        <v>23</v>
+      </c>
+      <c r="R2" s="39" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-3300-000000000000}"/>
-    <hyperlink ref="D3:D10" r:id="rId2" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-3300-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" xr:uid="{887B28E3-50F7-4F52-8B2E-5EF4187C1BC4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
-  <dimension ref="A1:A13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BAA440-EF09-47F4-83FC-456442901214}">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
+  <cols>
+    <col min="3" max="3" width="25.59765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.59765625" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.19921875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.8984375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:14">
       <c r="A1" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1">
+        <v>408</v>
+      </c>
+      <c r="B1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>396</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" t="s">
+        <v>221</v>
+      </c>
+      <c r="I1" t="s">
+        <v>61</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>215</v>
+      </c>
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" ht="17.399999999999999">
       <c r="A2" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1">
-      <c r="A3" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1">
-      <c r="A4" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1">
-      <c r="A5" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1">
-      <c r="A6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" t="s">
-        <v>188</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1">
-      <c r="A10" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" t="s">
-        <v>192</v>
+        <v>362</v>
+      </c>
+      <c r="B2" t="s">
+        <v>395</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>411</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>359</v>
+      </c>
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>407</v>
+      </c>
+      <c r="H2" s="16">
+        <v>1</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="J2" s="2">
+        <v>9000</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>388</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="N2" s="11" t="s">
+        <v>385</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{40F20844-5117-47D6-BE5F-527AE99DDF41}"/>
+    <hyperlink ref="C2" r:id="rId2" display="chsqanew02@mailinator.com" xr:uid="{FD08E511-44B9-452F-B1A8-4D73F23D4B51}"/>
+    <hyperlink ref="D2" r:id="rId3" display="chsqanew02@mailinator.com" xr:uid="{6A3AE5FB-D30B-47A6-9922-6BB5284DC178}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -9491,6 +9277,692 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-3200-000000000000}"/>
+    <hyperlink ref="A3" r:id="rId2" display="testconsultant3@mailinator.com" xr:uid="{00000000-0004-0000-3200-000001000000}"/>
+    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-3200-000002000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
+  <dimension ref="A1:Q10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <cols>
+    <col min="1" max="1" width="11" style="30"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17">
+      <c r="A1" s="30" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D1" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H1" t="s">
+        <v>62</v>
+      </c>
+      <c r="I1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" t="s">
+        <v>44</v>
+      </c>
+      <c r="L1" t="s">
+        <v>65</v>
+      </c>
+      <c r="M1" t="s">
+        <v>46</v>
+      </c>
+      <c r="N1" t="s">
+        <v>47</v>
+      </c>
+      <c r="O1" t="s">
+        <v>48</v>
+      </c>
+      <c r="P1" t="s">
+        <v>49</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17.399999999999999">
+      <c r="A2" s="31" t="s">
+        <v>285</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>123</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F2" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N2" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="17.399999999999999">
+      <c r="A3" s="31" t="s">
+        <v>342</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N3" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O3" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P3" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q3" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" ht="17.399999999999999">
+      <c r="A4" s="31" t="s">
+        <v>343</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E4" t="s">
+        <v>66</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" t="s">
+        <v>69</v>
+      </c>
+      <c r="I4" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K4" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L4" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N4" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O4" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P4" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q4" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="17.399999999999999">
+      <c r="A5" s="31" t="s">
+        <v>344</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="C5" t="s">
+        <v>174</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E5" t="s">
+        <v>66</v>
+      </c>
+      <c r="F5" t="s">
+        <v>67</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" t="s">
+        <v>69</v>
+      </c>
+      <c r="I5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N5" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P5" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q5" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="17.399999999999999">
+      <c r="A6" s="31" t="s">
+        <v>345</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E6" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H6" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" t="s">
+        <v>69</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K6" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M6" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O6" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P6" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q6" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="17.399999999999999">
+      <c r="A7" s="31" t="s">
+        <v>346</v>
+      </c>
+      <c r="B7" t="s">
+        <v>169</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E7" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H7" t="s">
+        <v>69</v>
+      </c>
+      <c r="I7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M7" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N7" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P7" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q7" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="17.399999999999999">
+      <c r="A8" s="31" t="s">
+        <v>347</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>170</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H8" t="s">
+        <v>69</v>
+      </c>
+      <c r="I8" t="s">
+        <v>69</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K8" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L8" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M8" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N8" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O8" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P8" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q8" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="17.399999999999999">
+      <c r="A9" s="31" t="s">
+        <v>348</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>171</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H9" t="s">
+        <v>69</v>
+      </c>
+      <c r="I9" t="s">
+        <v>69</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L9" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N9" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O9" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P9" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q9" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="17.399999999999999">
+      <c r="A10" s="31" t="s">
+        <v>349</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="C10" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="E10" t="s">
+        <v>66</v>
+      </c>
+      <c r="F10" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" t="s">
+        <v>69</v>
+      </c>
+      <c r="I10" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K10" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="N10" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="P10" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q10" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D2" r:id="rId1" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-3300-000000000000}"/>
+    <hyperlink ref="D3:D10" r:id="rId2" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-3300-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
+  <dimension ref="A1:A13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>192</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AB2"/>
@@ -9690,7 +10162,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -9809,7 +10281,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -9928,7 +10400,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10119,7 +10591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10310,7 +10782,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10501,7 +10973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10687,579 +11159,6 @@
   <hyperlinks>
     <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3B00-000000000000}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3B00-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
-  <dimension ref="A1:AB2"/>
-  <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="U1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="X1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="1" t="s">
-        <v>207</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2333</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>237</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3C00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3C00-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
-  <dimension ref="A1:AB2"/>
-  <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="U1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="X1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2333</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>236</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3D00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3D00-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
-  <dimension ref="A1:AB2"/>
-  <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="U1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="X1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2333</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>235</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3E00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3E00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11345,6 +11244,579 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2333</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3C00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3C00-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2333</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3D00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3D00-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2333</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3E00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3E00-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11535,7 +12007,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11726,7 +12198,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11917,7 +12389,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12108,7 +12580,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12299,7 +12771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12491,7 +12963,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12677,507 +13149,6 @@
   <hyperlinks>
     <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4500-000000000000}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4500-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
-  <dimension ref="A1:P2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:16">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>126</v>
-      </c>
-      <c r="F1" t="s">
-        <v>27</v>
-      </c>
-      <c r="G1" t="s">
-        <v>127</v>
-      </c>
-      <c r="H1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="I1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="J1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="K1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" t="s">
-        <v>45</v>
-      </c>
-      <c r="M1" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" t="s">
-        <v>48</v>
-      </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16">
-      <c r="A2" s="1" t="s">
-        <v>209</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>154</v>
-      </c>
-      <c r="D2" s="17" t="s">
-        <v>145</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>146</v>
-      </c>
-      <c r="F2" s="4">
-        <v>2200</v>
-      </c>
-      <c r="G2">
-        <v>2333</v>
-      </c>
-      <c r="H2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="I2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="K2" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="L2" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="M2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="O2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4600-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4600-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
-  <dimension ref="A1:AB2"/>
-  <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="U1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="X1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2333</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>242</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4700-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4700-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
-  <dimension ref="A1:AB2"/>
-  <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="U1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="X1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="1" t="s">
-        <v>211</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2333</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4800-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4800-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13268,6 +13239,507 @@
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>126</v>
+      </c>
+      <c r="F1" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" t="s">
+        <v>127</v>
+      </c>
+      <c r="H1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="I1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="J1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="K1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="L1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M1" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" t="s">
+        <v>48</v>
+      </c>
+      <c r="O1" t="s">
+        <v>49</v>
+      </c>
+      <c r="P1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16">
+      <c r="A2" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>154</v>
+      </c>
+      <c r="D2" s="17" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="F2" s="4">
+        <v>2200</v>
+      </c>
+      <c r="G2">
+        <v>2333</v>
+      </c>
+      <c r="H2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="I2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="L2" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="M2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="J2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4600-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4600-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2333</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4700-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4700-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2333</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4800-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4800-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -13386,7 +13858,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -13578,7 +14050,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -13769,7 +14241,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4C00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -13960,7 +14432,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4D00-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -14066,7 +14538,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4E00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -14118,7 +14590,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4F00-000000000000}">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:F2"/>
@@ -14178,51 +14650,6 @@
     <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-4F00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5000-000000000000}">
-  <sheetPr codeName="Sheet16"/>
-  <dimension ref="A1:D2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:4">
-      <c r="A1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" t="s">
-        <v>20</v>
-      </c>
-      <c r="C2" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -14306,4 +14733,49 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5000-000000000000}">
+  <sheetPr codeName="Sheet16"/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
pushing latest code till 6th Oct
</commit_message>
<xml_diff>
--- a/TestData/PartyLite_Smokes_Data.xlsx
+++ b/TestData/PartyLite_Smokes_Data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\PartyLiteAn (1)\PartyLiteAn\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\relite\partylite-test-automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3F9B829-89FE-4575-96AC-E37FE6CC6A1F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D353F97F-0AA4-47DE-AE4B-2E0D6824FD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="54" activeTab="56" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="54" activeTab="58" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddGuestDetails_PL" sheetId="17" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3400" uniqueCount="414">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3404" uniqueCount="417">
   <si>
     <t>Username</t>
   </si>
@@ -1337,9 +1337,6 @@
     <t>GB109_091LW6K</t>
   </si>
   <si>
-    <t>GC-15</t>
-  </si>
-  <si>
     <t>chsqanew02@mailinator.com</t>
   </si>
   <si>
@@ -1356,13 +1353,25 @@
   </si>
   <si>
     <t>test_smoke</t>
+  </si>
+  <si>
+    <t>SKU4</t>
+  </si>
+  <si>
+    <t>GC-20</t>
+  </si>
+  <si>
+    <t>gcno</t>
+  </si>
+  <si>
+    <t>gcpin</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1497,6 +1506,12 @@
     <font>
       <sz val="12"/>
       <color rgb="FF193157"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -8746,7 +8761,7 @@
         <v>359</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="D2" t="s">
         <v>362</v>
@@ -8814,7 +8829,7 @@
   </sheetPr>
   <dimension ref="A1:O2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
@@ -8888,10 +8903,10 @@
         <v>395</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="E2" s="36" t="s">
         <v>359</v>
@@ -8939,28 +8954,28 @@
 
 <file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABC2C4D-D525-4D71-9D7D-8F9EC67442AC}">
-  <dimension ref="A1:R2"/>
+  <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="1" max="3" width="8.796875" style="33"/>
-    <col min="4" max="4" width="4.19921875" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.69921875" style="33" customWidth="1"/>
-    <col min="6" max="6" width="18.69921875" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="9.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.59765625" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.796875" style="33"/>
-    <col min="11" max="11" width="11.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.796875" style="33"/>
+    <col min="1" max="4" width="8.796875" style="33"/>
+    <col min="5" max="5" width="4.19921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.69921875" style="33" customWidth="1"/>
+    <col min="7" max="7" width="18.69921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.59765625" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.796875" style="33"/>
+    <col min="12" max="12" width="11.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.796875" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18">
+    <row r="1" spans="1:19">
       <c r="A1" s="33" t="s">
         <v>397</v>
       </c>
@@ -8971,52 +8986,55 @@
         <v>400</v>
       </c>
       <c r="D1" s="33" t="s">
+        <v>413</v>
+      </c>
+      <c r="E1" s="33" t="s">
         <v>221</v>
       </c>
-      <c r="E1" s="33" t="s">
+      <c r="F1" s="33" t="s">
         <v>350</v>
       </c>
-      <c r="F1" s="33" t="s">
+      <c r="G1" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="33" t="s">
+      <c r="H1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="33" t="s">
+      <c r="I1" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="33" t="s">
+      <c r="J1" s="33" t="s">
         <v>61</v>
       </c>
-      <c r="J1" s="33" t="s">
+      <c r="K1" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="K1" s="33" t="s">
+      <c r="L1" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="L1" s="33" t="s">
+      <c r="M1" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="M1" s="33" t="s">
+      <c r="N1" s="33" t="s">
         <v>65</v>
       </c>
-      <c r="N1" s="33" t="s">
+      <c r="O1" s="33" t="s">
         <v>46</v>
       </c>
-      <c r="O1" s="33" t="s">
+      <c r="P1" s="33" t="s">
         <v>47</v>
       </c>
-      <c r="P1" s="33" t="s">
+      <c r="Q1" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="Q1" s="33" t="s">
+      <c r="R1" s="33" t="s">
         <v>49</v>
       </c>
-      <c r="R1" s="33" t="s">
+      <c r="S1" s="33" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.399999999999999">
+    <row r="2" spans="1:19" ht="17.399999999999999">
       <c r="A2" s="34" t="s">
         <v>398</v>
       </c>
@@ -9026,55 +9044,59 @@
       <c r="C2" s="34" t="s">
         <v>289</v>
       </c>
-      <c r="D2" s="35">
+      <c r="D2" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="E2" s="35">
         <v>2</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="F2" s="32" t="s">
         <v>351</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="G2" s="36" t="s">
         <v>404</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="H2" s="32" t="s">
         <v>362</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="I2" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="J2" s="32" t="s">
         <v>402</v>
       </c>
-      <c r="J2" s="33" t="s">
+      <c r="K2" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="K2" s="40">
+      <c r="L2" s="40">
         <v>8832</v>
-      </c>
-      <c r="L2" s="32" t="s">
-        <v>403</v>
       </c>
       <c r="M2" s="32" t="s">
         <v>403</v>
       </c>
-      <c r="N2" s="37" t="s">
+      <c r="N2" s="32" t="s">
+        <v>403</v>
+      </c>
+      <c r="O2" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="O2" s="38" t="s">
+      <c r="P2" s="38" t="s">
         <v>118</v>
       </c>
-      <c r="P2" s="39" t="s">
+      <c r="Q2" s="39" t="s">
         <v>119</v>
       </c>
-      <c r="Q2" s="39">
+      <c r="R2" s="39">
         <v>23</v>
       </c>
-      <c r="R2" s="39" t="s">
+      <c r="S2" s="39" t="s">
         <v>51</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="21" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{887B28E3-50F7-4F52-8B2E-5EF4187C1BC4}"/>
+    <hyperlink ref="G2" r:id="rId1" xr:uid="{887B28E3-50F7-4F52-8B2E-5EF4187C1BC4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9082,108 +9104,123 @@
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BAA440-EF09-47F4-83FC-456442901214}">
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:P2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
-    <col min="3" max="3" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.59765625" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.796875" style="33"/>
+    <col min="3" max="4" width="9.19921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.19921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="8.796875" style="33"/>
+    <col min="11" max="11" width="15.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.796875" style="33"/>
+    <col min="15" max="15" width="11.8984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.796875" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
-      <c r="A1" t="s">
+    <row r="1" spans="1:16">
+      <c r="A1" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>416</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="17.399999999999999">
+      <c r="A2" s="33" t="s">
+        <v>362</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>395</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>410</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>359</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="H2" s="35">
+        <v>1</v>
+      </c>
+      <c r="I2" s="35">
+        <v>409776</v>
+      </c>
+      <c r="J2" s="35">
+        <v>714131</v>
+      </c>
+      <c r="K2" s="32" t="s">
         <v>408</v>
       </c>
-      <c r="B1" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>396</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" t="s">
-        <v>221</v>
-      </c>
-      <c r="I1" t="s">
-        <v>61</v>
-      </c>
-      <c r="J1" t="s">
-        <v>64</v>
-      </c>
-      <c r="K1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L1" t="s">
-        <v>215</v>
-      </c>
-      <c r="M1" t="s">
-        <v>65</v>
-      </c>
-      <c r="N1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" ht="17.399999999999999">
-      <c r="A2" t="s">
-        <v>362</v>
-      </c>
-      <c r="B2" t="s">
-        <v>395</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>411</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>359</v>
-      </c>
-      <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>407</v>
-      </c>
-      <c r="H2" s="16">
-        <v>1</v>
-      </c>
-      <c r="I2" s="2" t="s">
+      <c r="L2" s="32">
+        <v>9000</v>
+      </c>
+      <c r="M2" s="32" t="s">
         <v>409</v>
       </c>
-      <c r="J2" s="2">
-        <v>9000</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>410</v>
-      </c>
-      <c r="L2" s="2" t="s">
+      <c r="N2" s="32" t="s">
         <v>388</v>
       </c>
-      <c r="M2" s="2" t="s">
+      <c r="O2" s="32" t="s">
         <v>405</v>
       </c>
-      <c r="N2" s="11" t="s">
+      <c r="P2" s="37" t="s">
         <v>385</v>
       </c>
     </row>

</xml_diff>

<commit_message>
latest changes as on 23 Nov
</commit_message>
<xml_diff>
--- a/TestData/PartyLite_Smokes_Data.xlsx
+++ b/TestData/PartyLite_Smokes_Data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\relite\partylite-test-automation\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D353F97F-0AA4-47DE-AE4B-2E0D6824FD15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354C636D-8647-48C0-86EB-4BC944FE6FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="54" activeTab="58" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="53" activeTab="57" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddGuestDetails_PL" sheetId="17" r:id="rId1"/>
@@ -114,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3404" uniqueCount="417">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3406" uniqueCount="419">
   <si>
     <t>Username</t>
   </si>
@@ -1199,9 +1199,6 @@
     <t>test_smoke2109shashwat@mailinator.com</t>
   </si>
   <si>
-    <t>test_smoke2209shashwat@mailinator.com</t>
-  </si>
-  <si>
     <t>Shashwat</t>
   </si>
   <si>
@@ -1241,9 +1238,6 @@
     <t>Queensland</t>
   </si>
   <si>
-    <t>test_smoke2209guest@mailinator.com</t>
-  </si>
-  <si>
     <t>434 Dorcas St</t>
   </si>
   <si>
@@ -1268,9 +1262,6 @@
     <t>9876787612</t>
   </si>
   <si>
-    <t>test_smoke2309guestpwsauto@mailinator.com</t>
-  </si>
-  <si>
     <t>PayPal</t>
   </si>
   <si>
@@ -1328,15 +1319,9 @@
     <t>OBERWÖLZ</t>
   </si>
   <si>
-    <t>test_smoke1001shashwat@mailinator.com</t>
-  </si>
-  <si>
     <t>079 294 04 91</t>
   </si>
   <si>
-    <t>GB109_091LW6K</t>
-  </si>
-  <si>
     <t>chsqanew02@mailinator.com</t>
   </si>
   <si>
@@ -1365,6 +1350,27 @@
   </si>
   <si>
     <t>gcpin</t>
+  </si>
+  <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>CH</t>
+  </si>
+  <si>
+    <t>test_smoke1025guest@mailinator.com</t>
+  </si>
+  <si>
+    <t>test_smoke2510guest@mailinator.com</t>
+  </si>
+  <si>
+    <t>test_smoke1025guestpwsauto@mailinator.com</t>
+  </si>
+  <si>
+    <t>GB110_U3TXT75</t>
+  </si>
+  <si>
+    <t>test_smoke1025.12@mailinator.com</t>
   </si>
 </sst>
 </file>
@@ -8094,7 +8100,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -8229,7 +8235,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -8302,16 +8308,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>414</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>361</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>362</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="G2" t="s">
         <v>69</v>
@@ -8320,16 +8326,16 @@
         <v>69</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="K2" s="2" t="s">
         <v>365</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>366</v>
-      </c>
       <c r="L2" s="2" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>164</v>
@@ -8362,8 +8368,8 @@
   </sheetPr>
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="D1" sqref="A1:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -8431,16 +8437,16 @@
         <v>50</v>
       </c>
       <c r="R1" t="s">
+        <v>367</v>
+      </c>
+      <c r="S1" t="s">
         <v>368</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>369</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>370</v>
-      </c>
-      <c r="U1" t="s">
-        <v>371</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="17.399999999999999">
@@ -8451,16 +8457,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>375</v>
+        <v>415</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="G2" t="s">
         <v>69</v>
@@ -8472,13 +8478,13 @@
         <v>3205</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>164</v>
@@ -8496,13 +8502,13 @@
         <v>51</v>
       </c>
       <c r="R2" t="s">
+        <v>371</v>
+      </c>
+      <c r="S2" t="s">
         <v>372</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>373</v>
-      </c>
-      <c r="T2" t="s">
-        <v>374</v>
       </c>
       <c r="U2">
         <v>4680</v>
@@ -8525,7 +8531,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -8580,13 +8586,13 @@
         <v>65</v>
       </c>
       <c r="L1" s="33" t="s">
+        <v>378</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>379</v>
+      </c>
+      <c r="N1" s="33" t="s">
         <v>380</v>
-      </c>
-      <c r="M1" s="33" t="s">
-        <v>381</v>
-      </c>
-      <c r="N1" s="33" t="s">
-        <v>382</v>
       </c>
       <c r="O1" s="33" t="s">
         <v>46</v>
@@ -8612,16 +8618,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>384</v>
+        <v>416</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E2" s="32" t="s">
         <v>84</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="G2" s="33" t="s">
         <v>69</v>
@@ -8633,22 +8639,22 @@
         <v>77700</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="K2" s="32" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="L2" s="32" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="N2" s="32">
         <v>77700</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
       <c r="P2" s="38" t="s">
         <v>118</v>
@@ -8680,7 +8686,7 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -8702,10 +8708,10 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="D1" t="s">
-        <v>391</v>
+        <v>388</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -8755,16 +8761,16 @@
     </row>
     <row r="2" spans="1:19" ht="17.399999999999999">
       <c r="A2" s="1" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>359</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>412</v>
+        <v>407</v>
       </c>
       <c r="D2" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -8776,7 +8782,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>386</v>
+        <v>383</v>
       </c>
       <c r="I2" t="s">
         <v>69</v>
@@ -8788,10 +8794,10 @@
         <v>16928</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>387</v>
+        <v>384</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>71</v>
@@ -8830,7 +8836,7 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -8859,7 +8865,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>9</v>
@@ -8897,16 +8903,16 @@
     </row>
     <row r="2" spans="1:15" ht="17.399999999999999">
       <c r="A2" s="33" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>411</v>
+        <v>406</v>
       </c>
       <c r="E2" s="36" t="s">
         <v>359</v>
@@ -8921,25 +8927,25 @@
         <v>1</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>392</v>
+        <v>389</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>394</v>
+        <v>391</v>
       </c>
       <c r="K2" s="32" t="s">
-        <v>393</v>
+        <v>390</v>
       </c>
       <c r="L2" s="32" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="M2" s="32">
         <v>1923123457</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>406</v>
+        <v>417</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>385</v>
+        <v>382</v>
       </c>
     </row>
   </sheetData>
@@ -8956,8 +8962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABC2C4D-D525-4D71-9D7D-8F9EC67442AC}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K17" sqref="K17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -8977,16 +8983,16 @@
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="33" t="s">
+        <v>394</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="C1" s="33" t="s">
         <v>397</v>
       </c>
-      <c r="B1" s="33" t="s">
-        <v>399</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>400</v>
-      </c>
       <c r="D1" s="33" t="s">
-        <v>413</v>
+        <v>408</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>221</v>
@@ -9036,16 +9042,16 @@
     </row>
     <row r="2" spans="1:19" ht="17.399999999999999">
       <c r="A2" s="34" t="s">
+        <v>395</v>
+      </c>
+      <c r="B2" s="34" t="s">
         <v>398</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>401</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>289</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="E2" s="35">
         <v>2</v>
@@ -9054,16 +9060,16 @@
         <v>351</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>404</v>
+        <v>418</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="I2" s="32" t="s">
         <v>84</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
       <c r="K2" s="33" t="s">
         <v>69</v>
@@ -9072,10 +9078,10 @@
         <v>8832</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="N2" s="32" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="O2" s="37" t="s">
         <v>164</v>
@@ -9104,10 +9110,10 @@
 
 <file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BAA440-EF09-47F4-83FC-456442901214}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O7" sqref="O7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -9124,9 +9130,9 @@
     <col min="16" max="16384" width="8.796875" style="33"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="33" t="s">
-        <v>407</v>
+        <v>402</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>149</v>
@@ -9135,7 +9141,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>9</v>
@@ -9150,10 +9156,10 @@
         <v>221</v>
       </c>
       <c r="I1" s="33" t="s">
-        <v>415</v>
+        <v>410</v>
       </c>
       <c r="J1" s="33" t="s">
-        <v>416</v>
+        <v>411</v>
       </c>
       <c r="K1" s="33" t="s">
         <v>61</v>
@@ -9173,19 +9179,22 @@
       <c r="P1" s="33" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="2" spans="1:16" ht="17.399999999999999">
+      <c r="Q1" s="33" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" ht="17.399999999999999">
       <c r="A2" s="33" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>395</v>
+        <v>392</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>410</v>
+        <v>405</v>
       </c>
       <c r="E2" s="36" t="s">
         <v>359</v>
@@ -9194,7 +9203,7 @@
         <v>4</v>
       </c>
       <c r="G2" s="34" t="s">
-        <v>414</v>
+        <v>409</v>
       </c>
       <c r="H2" s="35">
         <v>1</v>
@@ -9202,26 +9211,27 @@
       <c r="I2" s="35">
         <v>409776</v>
       </c>
-      <c r="J2" s="35">
-        <v>714131</v>
-      </c>
+      <c r="J2" s="35"/>
       <c r="K2" s="32" t="s">
-        <v>408</v>
+        <v>403</v>
       </c>
       <c r="L2" s="32">
         <v>9000</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>409</v>
+        <v>404</v>
       </c>
       <c r="N2" s="32" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="O2" s="32" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="P2" s="37" t="s">
-        <v>385</v>
+        <v>382</v>
+      </c>
+      <c r="Q2" s="33" t="s">
+        <v>413</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Smoke Tc4 added to branch by saravanan
</commit_message>
<xml_diff>
--- a/TestData/PartyLite_Smokes_Data.xlsx
+++ b/TestData/PartyLite_Smokes_Data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Downloads\relite\partylite-test-automation\TestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Automation_PL\relite-partylite-test-automation-462d32aa2b21\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354C636D-8647-48C0-86EB-4BC944FE6FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E09C7E4-56BC-4BE1-84F2-DC491B2E254A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="53" activeTab="57" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="51" activeTab="53" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AddGuestDetails_PL" sheetId="17" r:id="rId1"/>
@@ -66,43 +66,44 @@
     <sheet name="CustomerOrder_PL" sheetId="22" r:id="rId51"/>
     <sheet name="Smoke_TestCase_2" sheetId="84" r:id="rId52"/>
     <sheet name="Smoke_TestCase_3" sheetId="86" r:id="rId53"/>
-    <sheet name="Smoke_TestCase_6" sheetId="87" r:id="rId54"/>
-    <sheet name="Smoke_TestCase_7" sheetId="88" r:id="rId55"/>
-    <sheet name="Smoke_TestCase_8" sheetId="89" r:id="rId56"/>
-    <sheet name="Smoke_TestCase_10" sheetId="90" r:id="rId57"/>
-    <sheet name="Smoke_TestCase_11" sheetId="91" r:id="rId58"/>
-    <sheet name="Smoke_TestCase_12" sheetId="92" r:id="rId59"/>
-    <sheet name="MyAccount_Email_PL" sheetId="71" r:id="rId60"/>
-    <sheet name="GuestOrder_GC_PL" sheetId="23" r:id="rId61"/>
-    <sheet name="CategoryURL_PL" sheetId="49" r:id="rId62"/>
-    <sheet name="PaperOrderCreationDetails_PL" sheetId="7" r:id="rId63"/>
-    <sheet name="CollectivePT_PL" sheetId="39" r:id="rId64"/>
-    <sheet name="CollectivePT_FR_PL" sheetId="73" r:id="rId65"/>
-    <sheet name="ClassicPT_PL" sheetId="35" r:id="rId66"/>
-    <sheet name="ClassicPT_FR_PL" sheetId="72" r:id="rId67"/>
-    <sheet name="PO_DB1_PL" sheetId="55" r:id="rId68"/>
-    <sheet name="PO_DB2_PL" sheetId="56" r:id="rId69"/>
-    <sheet name="PO_DB3_PL" sheetId="57" r:id="rId70"/>
-    <sheet name="PO_DB4_PL" sheetId="58" r:id="rId71"/>
-    <sheet name="PO_DB5_PL" sheetId="59" r:id="rId72"/>
-    <sheet name="PO_DB6_PL" sheetId="60" r:id="rId73"/>
-    <sheet name="PO_DB7_PL" sheetId="61" r:id="rId74"/>
-    <sheet name="PO_DB8_PL" sheetId="62" r:id="rId75"/>
-    <sheet name="FYSPT_PL" sheetId="40" r:id="rId76"/>
-    <sheet name="FYSPT_FR_PL" sheetId="74" r:id="rId77"/>
-    <sheet name="ClassicPTRC_PL" sheetId="41" r:id="rId78"/>
-    <sheet name="ClassicPT_SC_PL" sheetId="42" r:id="rId79"/>
-    <sheet name="CollectivePT_SC_PL" sheetId="43" r:id="rId80"/>
-    <sheet name="FYSPT_SC_PL" sheetId="44" r:id="rId81"/>
-    <sheet name="ClassicPT_SH_PL" sheetId="45" r:id="rId82"/>
-    <sheet name="CollectivePT_SH_PL" sheetId="46" r:id="rId83"/>
-    <sheet name="FYSPT_SH_PL" sheetId="47" r:id="rId84"/>
-    <sheet name="ClassicPTCA_PL" sheetId="64" r:id="rId85"/>
-    <sheet name="FYSPTCA_PL" sheetId="66" r:id="rId86"/>
-    <sheet name="ShareParty_PL" sheetId="48" r:id="rId87"/>
-    <sheet name="PartyContactCreationNano_PL" sheetId="24" r:id="rId88"/>
-    <sheet name="PreventDupeAcctCreation_PL" sheetId="3" r:id="rId89"/>
-    <sheet name="SearchConsultant_PL" sheetId="4" r:id="rId90"/>
+    <sheet name="Smoke_TestCase_4" sheetId="93" r:id="rId54"/>
+    <sheet name="Smoke_TestCase_6" sheetId="87" r:id="rId55"/>
+    <sheet name="Smoke_TestCase_7" sheetId="88" r:id="rId56"/>
+    <sheet name="Smoke_TestCase_8" sheetId="89" r:id="rId57"/>
+    <sheet name="Smoke_TestCase_10" sheetId="90" r:id="rId58"/>
+    <sheet name="Smoke_TestCase_11" sheetId="91" r:id="rId59"/>
+    <sheet name="Smoke_TestCase_12" sheetId="92" r:id="rId60"/>
+    <sheet name="MyAccount_Email_PL" sheetId="71" r:id="rId61"/>
+    <sheet name="GuestOrder_GC_PL" sheetId="23" r:id="rId62"/>
+    <sheet name="CategoryURL_PL" sheetId="49" r:id="rId63"/>
+    <sheet name="PaperOrderCreationDetails_PL" sheetId="7" r:id="rId64"/>
+    <sheet name="CollectivePT_PL" sheetId="39" r:id="rId65"/>
+    <sheet name="CollectivePT_FR_PL" sheetId="73" r:id="rId66"/>
+    <sheet name="ClassicPT_PL" sheetId="35" r:id="rId67"/>
+    <sheet name="ClassicPT_FR_PL" sheetId="72" r:id="rId68"/>
+    <sheet name="PO_DB1_PL" sheetId="55" r:id="rId69"/>
+    <sheet name="PO_DB2_PL" sheetId="56" r:id="rId70"/>
+    <sheet name="PO_DB3_PL" sheetId="57" r:id="rId71"/>
+    <sheet name="PO_DB4_PL" sheetId="58" r:id="rId72"/>
+    <sheet name="PO_DB5_PL" sheetId="59" r:id="rId73"/>
+    <sheet name="PO_DB6_PL" sheetId="60" r:id="rId74"/>
+    <sheet name="PO_DB7_PL" sheetId="61" r:id="rId75"/>
+    <sheet name="PO_DB8_PL" sheetId="62" r:id="rId76"/>
+    <sheet name="FYSPT_PL" sheetId="40" r:id="rId77"/>
+    <sheet name="FYSPT_FR_PL" sheetId="74" r:id="rId78"/>
+    <sheet name="ClassicPTRC_PL" sheetId="41" r:id="rId79"/>
+    <sheet name="ClassicPT_SC_PL" sheetId="42" r:id="rId80"/>
+    <sheet name="CollectivePT_SC_PL" sheetId="43" r:id="rId81"/>
+    <sheet name="FYSPT_SC_PL" sheetId="44" r:id="rId82"/>
+    <sheet name="ClassicPT_SH_PL" sheetId="45" r:id="rId83"/>
+    <sheet name="CollectivePT_SH_PL" sheetId="46" r:id="rId84"/>
+    <sheet name="FYSPT_SH_PL" sheetId="47" r:id="rId85"/>
+    <sheet name="ClassicPTCA_PL" sheetId="64" r:id="rId86"/>
+    <sheet name="FYSPTCA_PL" sheetId="66" r:id="rId87"/>
+    <sheet name="ShareParty_PL" sheetId="48" r:id="rId88"/>
+    <sheet name="PartyContactCreationNano_PL" sheetId="24" r:id="rId89"/>
+    <sheet name="PreventDupeAcctCreation_PL" sheetId="3" r:id="rId90"/>
+    <sheet name="SearchConsultant_PL" sheetId="4" r:id="rId91"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -114,7 +115,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3406" uniqueCount="419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3423" uniqueCount="421">
   <si>
     <t>Username</t>
   </si>
@@ -1199,6 +1200,9 @@
     <t>test_smoke2109shashwat@mailinator.com</t>
   </si>
   <si>
+    <t>test_smoke2209shashwat@mailinator.com</t>
+  </si>
+  <si>
     <t>Shashwat</t>
   </si>
   <si>
@@ -1238,6 +1242,9 @@
     <t>Queensland</t>
   </si>
   <si>
+    <t>test_smoke2209guest@mailinator.com</t>
+  </si>
+  <si>
     <t>434 Dorcas St</t>
   </si>
   <si>
@@ -1262,6 +1269,9 @@
     <t>9876787612</t>
   </si>
   <si>
+    <t>test_smoke2309guestpwsauto@mailinator.com</t>
+  </si>
+  <si>
     <t>PayPal</t>
   </si>
   <si>
@@ -1319,9 +1329,15 @@
     <t>OBERWÖLZ</t>
   </si>
   <si>
+    <t>test_smoke1001shashwat@mailinator.com</t>
+  </si>
+  <si>
     <t>079 294 04 91</t>
   </si>
   <si>
+    <t>GB109_091LW6K</t>
+  </si>
+  <si>
     <t>chsqanew02@mailinator.com</t>
   </si>
   <si>
@@ -1352,34 +1368,32 @@
     <t>gcpin</t>
   </si>
   <si>
-    <t>Country</t>
-  </si>
-  <si>
-    <t>CH</t>
-  </si>
-  <si>
-    <t>test_smoke1025guest@mailinator.com</t>
-  </si>
-  <si>
-    <t>test_smoke2510guest@mailinator.com</t>
-  </si>
-  <si>
-    <t>test_smoke1025guestpwsauto@mailinator.com</t>
-  </si>
-  <si>
-    <t>GB110_U3TXT75</t>
-  </si>
-  <si>
-    <t>test_smoke1025.12@mailinator.com</t>
+    <t>2 Topaz Crescent</t>
+  </si>
+  <si>
+    <t>Y1A 6B3</t>
+  </si>
+  <si>
+    <t>Whitehorse</t>
+  </si>
+  <si>
+    <t>Yukon Territory</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22">
+  <fonts count="23">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1542,18 +1556,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1561,35 +1574,39 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1912,10 +1929,10 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="35.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -2095,9 +2112,9 @@
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="5" max="5" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2177,7 +2194,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -2265,7 +2282,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="19.8">
+    <row r="2" spans="1:28" ht="19.5">
       <c r="A2" s="26" t="s">
         <v>248</v>
       </c>
@@ -2367,7 +2384,7 @@
       <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -2389,7 +2406,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20.399999999999999">
+    <row r="2" spans="1:6" ht="20">
       <c r="A2" s="12" t="s">
         <v>110</v>
       </c>
@@ -2409,7 +2426,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="25.2">
+    <row r="3" spans="1:6" ht="25.5">
       <c r="A3" s="15" t="s">
         <v>113</v>
       </c>
@@ -2442,7 +2459,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -2512,7 +2529,7 @@
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -2588,7 +2605,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -2652,7 +2669,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -2704,7 +2721,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -2756,7 +2773,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -2844,7 +2861,7 @@
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -2950,7 +2967,7 @@
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -3020,7 +3037,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.399999999999999">
+    <row r="5" spans="1:5" ht="17.5">
       <c r="A5" s="11" t="s">
         <v>105</v>
       </c>
@@ -3037,7 +3054,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.399999999999999">
+    <row r="6" spans="1:5" ht="17.5">
       <c r="A6" s="11" t="s">
         <v>300</v>
       </c>
@@ -3067,7 +3084,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -3126,7 +3143,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -3185,7 +3202,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -3281,11 +3298,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="35.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3369,7 +3386,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -3427,7 +3444,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.399999999999999">
+    <row r="2" spans="1:18" ht="17.5">
       <c r="A2" t="s">
         <v>217</v>
       </c>
@@ -3500,7 +3517,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -3691,7 +3708,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -3750,7 +3767,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -3779,10 +3796,10 @@
       <selection activeCell="F7" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.09765625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3844,10 +3861,10 @@
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="23.8984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.8984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.9140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -3903,7 +3920,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.399999999999999">
+    <row r="2" spans="1:17" ht="17.5">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -3973,7 +3990,7 @@
       <selection sqref="A1:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -4025,7 +4042,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17.399999999999999">
+    <row r="2" spans="1:16" ht="17.5">
       <c r="A2" s="16" t="s">
         <v>97</v>
       </c>
@@ -4092,10 +4109,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="35.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4106,7 +4123,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20.399999999999999">
+    <row r="2" spans="1:2" ht="20">
       <c r="A2" s="20" t="s">
         <v>162</v>
       </c>
@@ -4128,7 +4145,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -4254,7 +4271,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="3" max="3" width="28" customWidth="1"/>
   </cols>
@@ -4315,7 +4332,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.399999999999999">
+    <row r="2" spans="1:18" ht="17.5">
       <c r="A2" s="5" t="s">
         <v>332</v>
       </c>
@@ -4387,7 +4404,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4397,7 +4414,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.8">
+    <row r="2" spans="1:2" ht="16.5">
       <c r="A2" s="5" t="s">
         <v>285</v>
       </c>
@@ -4418,10 +4435,10 @@
       <selection activeCell="D2" sqref="D2:E79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="24.09765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.08203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -4435,7 +4452,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="16.8">
+    <row r="2" spans="1:5" ht="16.5">
       <c r="A2" t="s">
         <v>322</v>
       </c>
@@ -4452,7 +4469,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="16.8">
+    <row r="3" spans="1:5" ht="16.5">
       <c r="A3" t="s">
         <v>322</v>
       </c>
@@ -4469,7 +4486,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="16.8">
+    <row r="4" spans="1:5" ht="16.5">
       <c r="A4" t="s">
         <v>322</v>
       </c>
@@ -4486,7 +4503,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="16.8">
+    <row r="5" spans="1:5" ht="16.5">
       <c r="A5" t="s">
         <v>322</v>
       </c>
@@ -4503,7 +4520,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="16.8">
+    <row r="6" spans="1:5" ht="16.5">
       <c r="A6" t="s">
         <v>322</v>
       </c>
@@ -4520,7 +4537,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="16.8">
+    <row r="7" spans="1:5" ht="16.5">
       <c r="A7" t="s">
         <v>322</v>
       </c>
@@ -4537,7 +4554,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="16.8">
+    <row r="8" spans="1:5" ht="16.5">
       <c r="A8" t="s">
         <v>322</v>
       </c>
@@ -4554,7 +4571,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="16.8">
+    <row r="9" spans="1:5" ht="16.5">
       <c r="A9" t="s">
         <v>322</v>
       </c>
@@ -4571,7 +4588,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="16.8">
+    <row r="10" spans="1:5" ht="16.5">
       <c r="A10" t="s">
         <v>322</v>
       </c>
@@ -4588,7 +4605,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="16.8">
+    <row r="11" spans="1:5" ht="16.5">
       <c r="A11" t="s">
         <v>322</v>
       </c>
@@ -4605,7 +4622,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="16.8">
+    <row r="12" spans="1:5" ht="16.5">
       <c r="A12" t="s">
         <v>322</v>
       </c>
@@ -4622,7 +4639,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="16.8">
+    <row r="13" spans="1:5" ht="16.5">
       <c r="A13" t="s">
         <v>322</v>
       </c>
@@ -4639,7 +4656,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="16.8">
+    <row r="14" spans="1:5" ht="16.5">
       <c r="A14" t="s">
         <v>322</v>
       </c>
@@ -4656,7 +4673,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="16.8">
+    <row r="15" spans="1:5" ht="16.5">
       <c r="A15" t="s">
         <v>322</v>
       </c>
@@ -4673,7 +4690,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="16.8">
+    <row r="16" spans="1:5" ht="16.5">
       <c r="A16" t="s">
         <v>322</v>
       </c>
@@ -4690,7 +4707,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="16.8">
+    <row r="17" spans="1:5" ht="16.5">
       <c r="A17" t="s">
         <v>322</v>
       </c>
@@ -4707,7 +4724,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="18" spans="1:5" ht="16.8">
+    <row r="18" spans="1:5" ht="16.5">
       <c r="A18" t="s">
         <v>322</v>
       </c>
@@ -4724,7 +4741,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="16.8">
+    <row r="19" spans="1:5" ht="16.5">
       <c r="A19" t="s">
         <v>322</v>
       </c>
@@ -4741,7 +4758,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="20" spans="1:5" ht="16.8">
+    <row r="20" spans="1:5" ht="16.5">
       <c r="A20" t="s">
         <v>322</v>
       </c>
@@ -4758,7 +4775,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="16.8">
+    <row r="21" spans="1:5" ht="16.5">
       <c r="A21" t="s">
         <v>322</v>
       </c>
@@ -4775,7 +4792,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="22" spans="1:5" ht="16.8">
+    <row r="22" spans="1:5" ht="16.5">
       <c r="D22" t="s">
         <v>304</v>
       </c>
@@ -4783,7 +4800,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="23" spans="1:5" ht="16.8">
+    <row r="23" spans="1:5" ht="16.5">
       <c r="D23" t="s">
         <v>305</v>
       </c>
@@ -4791,7 +4808,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="24" spans="1:5" ht="16.8">
+    <row r="24" spans="1:5" ht="16.5">
       <c r="D24" t="s">
         <v>306</v>
       </c>
@@ -4799,7 +4816,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="25" spans="1:5" ht="16.8">
+    <row r="25" spans="1:5" ht="16.5">
       <c r="D25" t="s">
         <v>307</v>
       </c>
@@ -4807,7 +4824,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="16.8">
+    <row r="26" spans="1:5" ht="16.5">
       <c r="D26" t="s">
         <v>308</v>
       </c>
@@ -4815,7 +4832,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="27" spans="1:5" ht="16.8">
+    <row r="27" spans="1:5" ht="16.5">
       <c r="D27" t="s">
         <v>309</v>
       </c>
@@ -4823,7 +4840,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:5" ht="16.8">
+    <row r="28" spans="1:5" ht="16.5">
       <c r="D28" t="s">
         <v>310</v>
       </c>
@@ -4831,7 +4848,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="29" spans="1:5" ht="16.8">
+    <row r="29" spans="1:5" ht="16.5">
       <c r="D29" t="s">
         <v>311</v>
       </c>
@@ -4839,7 +4856,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="30" spans="1:5" ht="16.8">
+    <row r="30" spans="1:5" ht="16.5">
       <c r="D30" t="s">
         <v>312</v>
       </c>
@@ -4847,7 +4864,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:5" ht="16.8">
+    <row r="31" spans="1:5" ht="16.5">
       <c r="D31" t="s">
         <v>313</v>
       </c>
@@ -4855,7 +4872,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="16.8">
+    <row r="32" spans="1:5" ht="16.5">
       <c r="D32" t="s">
         <v>253</v>
       </c>
@@ -4863,7 +4880,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="33" spans="4:5" ht="16.8">
+    <row r="33" spans="4:5" ht="16.5">
       <c r="D33" t="s">
         <v>314</v>
       </c>
@@ -4871,7 +4888,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="34" spans="4:5" ht="16.8">
+    <row r="34" spans="4:5" ht="16.5">
       <c r="D34" t="s">
         <v>315</v>
       </c>
@@ -4879,7 +4896,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="35" spans="4:5" ht="16.8">
+    <row r="35" spans="4:5" ht="16.5">
       <c r="D35" t="s">
         <v>316</v>
       </c>
@@ -4887,7 +4904,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="36" spans="4:5" ht="16.8">
+    <row r="36" spans="4:5" ht="16.5">
       <c r="D36" t="s">
         <v>317</v>
       </c>
@@ -4895,7 +4912,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="37" spans="4:5" ht="16.8">
+    <row r="37" spans="4:5" ht="16.5">
       <c r="D37" t="s">
         <v>318</v>
       </c>
@@ -4903,7 +4920,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="38" spans="4:5" ht="16.8">
+    <row r="38" spans="4:5" ht="16.5">
       <c r="D38" t="s">
         <v>319</v>
       </c>
@@ -4911,7 +4928,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="39" spans="4:5" ht="16.8">
+    <row r="39" spans="4:5" ht="16.5">
       <c r="D39" t="s">
         <v>320</v>
       </c>
@@ -4919,7 +4936,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="40" spans="4:5" ht="16.8">
+    <row r="40" spans="4:5" ht="16.5">
       <c r="D40" s="5" t="s">
         <v>285</v>
       </c>
@@ -4927,7 +4944,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="41" spans="4:5" ht="16.8">
+    <row r="41" spans="4:5" ht="16.5">
       <c r="D41" t="s">
         <v>303</v>
       </c>
@@ -4935,7 +4952,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="42" spans="4:5" ht="16.8">
+    <row r="42" spans="4:5" ht="16.5">
       <c r="D42" t="s">
         <v>304</v>
       </c>
@@ -4943,7 +4960,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="43" spans="4:5" ht="16.8">
+    <row r="43" spans="4:5" ht="16.5">
       <c r="D43" t="s">
         <v>305</v>
       </c>
@@ -4951,7 +4968,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="44" spans="4:5" ht="16.8">
+    <row r="44" spans="4:5" ht="16.5">
       <c r="D44" t="s">
         <v>306</v>
       </c>
@@ -4959,7 +4976,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="45" spans="4:5" ht="16.8">
+    <row r="45" spans="4:5" ht="16.5">
       <c r="D45" t="s">
         <v>307</v>
       </c>
@@ -4967,7 +4984,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="46" spans="4:5" ht="16.8">
+    <row r="46" spans="4:5" ht="16.5">
       <c r="D46" t="s">
         <v>308</v>
       </c>
@@ -4975,7 +4992,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="47" spans="4:5" ht="16.8">
+    <row r="47" spans="4:5" ht="16.5">
       <c r="D47" t="s">
         <v>309</v>
       </c>
@@ -4983,7 +5000,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="48" spans="4:5" ht="16.8">
+    <row r="48" spans="4:5" ht="16.5">
       <c r="D48" t="s">
         <v>310</v>
       </c>
@@ -4991,7 +5008,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="49" spans="4:5" ht="16.8">
+    <row r="49" spans="4:5" ht="16.5">
       <c r="D49" t="s">
         <v>311</v>
       </c>
@@ -4999,7 +5016,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="50" spans="4:5" ht="16.8">
+    <row r="50" spans="4:5" ht="16.5">
       <c r="D50" t="s">
         <v>312</v>
       </c>
@@ -5007,7 +5024,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="51" spans="4:5" ht="16.8">
+    <row r="51" spans="4:5" ht="16.5">
       <c r="D51" t="s">
         <v>313</v>
       </c>
@@ -5015,7 +5032,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="52" spans="4:5" ht="16.8">
+    <row r="52" spans="4:5" ht="16.5">
       <c r="D52" t="s">
         <v>253</v>
       </c>
@@ -5023,7 +5040,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="53" spans="4:5" ht="16.8">
+    <row r="53" spans="4:5" ht="16.5">
       <c r="D53" t="s">
         <v>314</v>
       </c>
@@ -5031,7 +5048,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="54" spans="4:5" ht="16.8">
+    <row r="54" spans="4:5" ht="16.5">
       <c r="D54" t="s">
         <v>315</v>
       </c>
@@ -5039,7 +5056,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="55" spans="4:5" ht="16.8">
+    <row r="55" spans="4:5" ht="16.5">
       <c r="D55" t="s">
         <v>316</v>
       </c>
@@ -5047,7 +5064,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="56" spans="4:5" ht="16.8">
+    <row r="56" spans="4:5" ht="16.5">
       <c r="D56" t="s">
         <v>317</v>
       </c>
@@ -5055,7 +5072,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="57" spans="4:5" ht="16.8">
+    <row r="57" spans="4:5" ht="16.5">
       <c r="D57" t="s">
         <v>318</v>
       </c>
@@ -5063,7 +5080,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="4:5" ht="16.8">
+    <row r="58" spans="4:5" ht="16.5">
       <c r="D58" t="s">
         <v>319</v>
       </c>
@@ -5071,7 +5088,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="59" spans="4:5" ht="16.8">
+    <row r="59" spans="4:5" ht="16.5">
       <c r="D59" t="s">
         <v>320</v>
       </c>
@@ -5079,7 +5096,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="60" spans="4:5" ht="16.8">
+    <row r="60" spans="4:5" ht="16.5">
       <c r="D60" s="5" t="s">
         <v>285</v>
       </c>
@@ -5087,7 +5104,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="61" spans="4:5" ht="16.8">
+    <row r="61" spans="4:5" ht="16.5">
       <c r="D61" t="s">
         <v>303</v>
       </c>
@@ -5095,7 +5112,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="62" spans="4:5" ht="16.8">
+    <row r="62" spans="4:5" ht="16.5">
       <c r="D62" t="s">
         <v>304</v>
       </c>
@@ -5103,7 +5120,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="63" spans="4:5" ht="16.8">
+    <row r="63" spans="4:5" ht="16.5">
       <c r="D63" t="s">
         <v>305</v>
       </c>
@@ -5111,7 +5128,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="64" spans="4:5" ht="16.8">
+    <row r="64" spans="4:5" ht="16.5">
       <c r="D64" t="s">
         <v>306</v>
       </c>
@@ -5119,7 +5136,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="65" spans="4:5" ht="16.8">
+    <row r="65" spans="4:5" ht="16.5">
       <c r="D65" t="s">
         <v>307</v>
       </c>
@@ -5127,7 +5144,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="66" spans="4:5" ht="16.8">
+    <row r="66" spans="4:5" ht="16.5">
       <c r="D66" t="s">
         <v>308</v>
       </c>
@@ -5135,7 +5152,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="67" spans="4:5" ht="16.8">
+    <row r="67" spans="4:5" ht="16.5">
       <c r="D67" t="s">
         <v>309</v>
       </c>
@@ -5143,7 +5160,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="68" spans="4:5" ht="16.8">
+    <row r="68" spans="4:5" ht="16.5">
       <c r="D68" t="s">
         <v>310</v>
       </c>
@@ -5151,7 +5168,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="69" spans="4:5" ht="16.8">
+    <row r="69" spans="4:5" ht="16.5">
       <c r="D69" t="s">
         <v>311</v>
       </c>
@@ -5159,7 +5176,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="70" spans="4:5" ht="16.8">
+    <row r="70" spans="4:5" ht="16.5">
       <c r="D70" t="s">
         <v>312</v>
       </c>
@@ -5167,7 +5184,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="71" spans="4:5" ht="16.8">
+    <row r="71" spans="4:5" ht="16.5">
       <c r="D71" t="s">
         <v>313</v>
       </c>
@@ -5175,7 +5192,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="72" spans="4:5" ht="16.8">
+    <row r="72" spans="4:5" ht="16.5">
       <c r="D72" t="s">
         <v>253</v>
       </c>
@@ -5183,7 +5200,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="73" spans="4:5" ht="16.8">
+    <row r="73" spans="4:5" ht="16.5">
       <c r="D73" t="s">
         <v>314</v>
       </c>
@@ -5191,7 +5208,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="74" spans="4:5" ht="16.8">
+    <row r="74" spans="4:5" ht="16.5">
       <c r="D74" t="s">
         <v>315</v>
       </c>
@@ -5199,7 +5216,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="4:5" ht="16.8">
+    <row r="75" spans="4:5" ht="16.5">
       <c r="D75" t="s">
         <v>316</v>
       </c>
@@ -5207,7 +5224,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="76" spans="4:5" ht="16.8">
+    <row r="76" spans="4:5" ht="16.5">
       <c r="D76" t="s">
         <v>317</v>
       </c>
@@ -5215,7 +5232,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="77" spans="4:5" ht="16.8">
+    <row r="77" spans="4:5" ht="16.5">
       <c r="D77" t="s">
         <v>318</v>
       </c>
@@ -5223,7 +5240,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="78" spans="4:5" ht="16.8">
+    <row r="78" spans="4:5" ht="16.5">
       <c r="D78" t="s">
         <v>319</v>
       </c>
@@ -5231,7 +5248,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="79" spans="4:5" ht="16.8">
+    <row r="79" spans="4:5" ht="16.5">
       <c r="D79" t="s">
         <v>320</v>
       </c>
@@ -5252,7 +5269,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5262,7 +5279,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="16.8">
+    <row r="2" spans="1:2" ht="16.5">
       <c r="A2" s="29" t="s">
         <v>339</v>
       </c>
@@ -5284,7 +5301,7 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -5339,7 +5356,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.399999999999999">
+    <row r="2" spans="1:17" ht="17.5">
       <c r="A2" s="5" t="s">
         <v>287</v>
       </c>
@@ -5392,7 +5409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.399999999999999">
+    <row r="3" spans="1:17" ht="17.5">
       <c r="A3" s="5" t="s">
         <v>288</v>
       </c>
@@ -5445,7 +5462,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.399999999999999">
+    <row r="4" spans="1:17" ht="17.5">
       <c r="A4" s="5" t="s">
         <v>289</v>
       </c>
@@ -5498,7 +5515,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.399999999999999">
+    <row r="5" spans="1:17" ht="17.5">
       <c r="A5" s="5" t="s">
         <v>285</v>
       </c>
@@ -5551,7 +5568,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="20.399999999999999">
+    <row r="6" spans="1:17" ht="20">
       <c r="A6" s="13" t="s">
         <v>293</v>
       </c>
@@ -5624,9 +5641,9 @@
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="3" max="3" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5685,7 +5702,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.399999999999999">
+    <row r="2" spans="1:18" ht="17.5">
       <c r="A2" s="5" t="s">
         <v>289</v>
       </c>
@@ -5741,7 +5758,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.399999999999999">
+    <row r="3" spans="1:18" ht="17.5">
       <c r="A3" s="5" t="s">
         <v>288</v>
       </c>
@@ -5797,7 +5814,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17.399999999999999">
+    <row r="4" spans="1:18" ht="17.5">
       <c r="A4" s="5" t="s">
         <v>289</v>
       </c>
@@ -5853,7 +5870,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.399999999999999">
+    <row r="5" spans="1:18" ht="17.5">
       <c r="A5" s="5" t="s">
         <v>285</v>
       </c>
@@ -5909,7 +5926,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="20.399999999999999">
+    <row r="6" spans="1:18" ht="20">
       <c r="A6" s="13" t="s">
         <v>293</v>
       </c>
@@ -5985,7 +6002,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -6339,7 +6356,7 @@
       <selection activeCell="D2" sqref="D2:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -6796,7 +6813,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -6848,7 +6865,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17.399999999999999">
+    <row r="2" spans="1:16" ht="17.5">
       <c r="A2" s="16" t="s">
         <v>95</v>
       </c>
@@ -6915,7 +6932,7 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -6950,7 +6967,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
@@ -6999,7 +7016,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17.399999999999999">
+    <row r="2" spans="1:15" ht="17.5">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -7059,7 +7076,7 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -7114,7 +7131,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.399999999999999">
+    <row r="2" spans="1:17" ht="17.5">
       <c r="A2" t="s">
         <v>194</v>
       </c>
@@ -7180,7 +7197,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -7223,7 +7240,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17.399999999999999">
+    <row r="2" spans="1:13" ht="17.5">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -7278,10 +7295,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="9" max="9" width="11.09765625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -7419,9 +7436,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="6" max="6" width="20.59765625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.58203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -7482,7 +7499,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -7542,7 +7559,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -7661,7 +7678,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -7714,7 +7731,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -7766,7 +7783,7 @@
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -7821,7 +7838,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.399999999999999">
+    <row r="2" spans="1:17" ht="17.5">
       <c r="A2" s="5" t="s">
         <v>253</v>
       </c>
@@ -7891,7 +7908,7 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -7961,9 +7978,9 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -8019,7 +8036,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.399999999999999">
+    <row r="2" spans="1:17" ht="17.5">
       <c r="A2" s="1" t="s">
         <v>353</v>
       </c>
@@ -8100,15 +8117,15 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="18.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.4140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8165,7 +8182,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.399999999999999">
+    <row r="2" spans="1:17" ht="17.5">
       <c r="A2" s="1" t="s">
         <v>360</v>
       </c>
@@ -8235,16 +8252,16 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="3" max="3" width="18.69921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.69921875" customWidth="1"/>
-    <col min="6" max="6" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.6640625" customWidth="1"/>
+    <col min="6" max="6" width="15.4140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -8300,7 +8317,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.399999999999999">
+    <row r="2" spans="1:17" ht="17.5">
       <c r="A2" s="5" t="s">
         <v>354</v>
       </c>
@@ -8308,16 +8325,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>414</v>
+        <v>361</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="G2" t="s">
         <v>69</v>
@@ -8326,16 +8343,16 @@
         <v>69</v>
       </c>
       <c r="I2" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="J2" s="2" t="s">
-        <v>363</v>
-      </c>
       <c r="K2" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>164</v>
@@ -8362,26 +8379,120 @@
 </file>
 
 <file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34C2D9A-3197-4887-BB87-C55FC188EBDB}">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.4140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.9140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.58203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.4140625" style="41" customWidth="1"/>
+    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.75" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>417</v>
+      </c>
+      <c r="C2" t="s">
+        <v>418</v>
+      </c>
+      <c r="D2" t="s">
+        <v>419</v>
+      </c>
+      <c r="E2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F2" t="s">
+        <v>420</v>
+      </c>
+      <c r="G2" s="42" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2">
+        <v>23</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377BF7CB-F633-49F4-8D49-EB8446EAC16C}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:U2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="2" max="2" width="4.19921875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.59765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.3984375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.296875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.8984375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.8984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.4140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.9140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.9140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -8437,19 +8548,19 @@
         <v>50</v>
       </c>
       <c r="R1" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="S1" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="T1" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="U1" t="s">
-        <v>370</v>
-      </c>
-    </row>
-    <row r="2" spans="1:21" ht="17.399999999999999">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" ht="17.5">
       <c r="A2" s="5" t="s">
         <v>354</v>
       </c>
@@ -8457,16 +8568,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>415</v>
+        <v>375</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>84</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="G2" t="s">
         <v>69</v>
@@ -8478,18 +8589,18 @@
         <v>3205</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="M2" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="43" t="s">
         <v>118</v>
       </c>
       <c r="O2" s="4" t="s">
@@ -8502,13 +8613,13 @@
         <v>51</v>
       </c>
       <c r="R2" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="S2" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="T2" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="U2">
         <v>4680</v>
@@ -8523,7 +8634,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E84195DF-01B2-4D45-8E2B-90A4FB63FF02}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -8531,24 +8642,24 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="8.796875" style="33"/>
-    <col min="2" max="2" width="4.19921875" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.69921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.83203125" style="33"/>
+    <col min="2" max="2" width="4.1640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" style="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.59765625" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.3984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.796875" style="33"/>
-    <col min="9" max="9" width="7.296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.296875" style="33" customWidth="1"/>
-    <col min="12" max="12" width="18.296875" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.58203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.4140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.83203125" style="33"/>
+    <col min="9" max="9" width="7.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" style="33" customWidth="1"/>
+    <col min="12" max="12" width="18.33203125" style="33" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.796875" style="33"/>
+    <col min="14" max="16384" width="8.83203125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -8586,13 +8697,13 @@
         <v>65</v>
       </c>
       <c r="L1" s="33" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="M1" s="33" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="N1" s="33" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="O1" s="33" t="s">
         <v>46</v>
@@ -8610,7 +8721,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="17.399999999999999">
+    <row r="2" spans="1:19" ht="17.5">
       <c r="A2" s="34" t="s">
         <v>354</v>
       </c>
@@ -8618,16 +8729,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>416</v>
+        <v>384</v>
       </c>
       <c r="D2" s="32" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E2" s="32" t="s">
         <v>84</v>
       </c>
       <c r="F2" s="32" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="G2" s="33" t="s">
         <v>69</v>
@@ -8639,22 +8750,22 @@
         <v>77700</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="K2" s="32" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="L2" s="32" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="N2" s="32">
         <v>77700</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
       <c r="P2" s="38" t="s">
         <v>118</v>
@@ -8678,7 +8789,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622CFA83-E905-4467-BCFD-8E7E2CF53AA9}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -8686,17 +8797,17 @@
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="25.59765625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.58203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.4140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.3984375" customWidth="1"/>
-    <col min="5" max="5" width="20.19921875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.4140625" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.4140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8708,10 +8819,10 @@
         <v>9</v>
       </c>
       <c r="C1" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="D1" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="E1" t="s">
         <v>3</v>
@@ -8759,18 +8870,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="17.399999999999999">
+    <row r="2" spans="1:19" ht="17.5">
       <c r="A2" s="1" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>359</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>407</v>
+        <v>412</v>
       </c>
       <c r="D2" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E2" t="s">
         <v>4</v>
@@ -8782,7 +8893,7 @@
         <v>1</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>383</v>
+        <v>386</v>
       </c>
       <c r="I2" t="s">
         <v>69</v>
@@ -8794,10 +8905,10 @@
         <v>16928</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>384</v>
+        <v>387</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>71</v>
@@ -8828,7 +8939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9962DFF2-70D3-42DF-A705-EB69D22B5F41}">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
@@ -8836,22 +8947,22 @@
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="2" width="8.796875" style="33"/>
-    <col min="3" max="4" width="9.296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.19921875" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.796875" style="33"/>
-    <col min="9" max="9" width="15.3984375" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.83203125" style="33"/>
+    <col min="3" max="4" width="9.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.4140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.83203125" style="33"/>
+    <col min="9" max="9" width="15.4140625" style="33" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.796875" style="33"/>
-    <col min="13" max="13" width="11.8984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.8984375" style="33" customWidth="1"/>
-    <col min="15" max="16384" width="8.796875" style="33"/>
+    <col min="11" max="12" width="8.83203125" style="33"/>
+    <col min="13" max="13" width="11.9140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.9140625" style="33" customWidth="1"/>
+    <col min="15" max="16384" width="8.83203125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -8865,7 +8976,7 @@
         <v>7</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>393</v>
+        <v>396</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>9</v>
@@ -8901,18 +9012,18 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17.399999999999999">
+    <row r="2" spans="1:15" ht="17.5">
       <c r="A2" s="33" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="B2" s="33" t="s">
-        <v>392</v>
+        <v>395</v>
       </c>
       <c r="C2" s="36" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="D2" s="36" t="s">
-        <v>406</v>
+        <v>411</v>
       </c>
       <c r="E2" s="36" t="s">
         <v>359</v>
@@ -8927,25 +9038,25 @@
         <v>1</v>
       </c>
       <c r="I2" s="32" t="s">
-        <v>389</v>
+        <v>392</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>391</v>
+        <v>394</v>
       </c>
       <c r="K2" s="32" t="s">
-        <v>390</v>
+        <v>393</v>
       </c>
       <c r="L2" s="32" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="M2" s="32">
         <v>1923123457</v>
       </c>
       <c r="N2" s="33" t="s">
-        <v>417</v>
+        <v>406</v>
       </c>
       <c r="O2" s="37" t="s">
-        <v>382</v>
+        <v>385</v>
       </c>
     </row>
   </sheetData>
@@ -8958,41 +9069,41 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABC2C4D-D525-4D71-9D7D-8F9EC67442AC}">
   <dimension ref="A1:S2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="4" width="8.796875" style="33"/>
-    <col min="5" max="5" width="4.19921875" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.69921875" style="33" customWidth="1"/>
-    <col min="7" max="7" width="18.69921875" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="8.83203125" style="33"/>
+    <col min="5" max="5" width="4.1640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" style="33" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.59765625" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.3984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.796875" style="33"/>
+    <col min="9" max="9" width="8.58203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.4140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.83203125" style="33"/>
     <col min="12" max="12" width="11.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.296875" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.796875" style="33"/>
+    <col min="13" max="13" width="12.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.83203125" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
       <c r="A1" s="33" t="s">
-        <v>394</v>
+        <v>397</v>
       </c>
       <c r="B1" s="33" t="s">
-        <v>396</v>
+        <v>399</v>
       </c>
       <c r="C1" s="33" t="s">
-        <v>397</v>
+        <v>400</v>
       </c>
       <c r="D1" s="33" t="s">
-        <v>408</v>
+        <v>413</v>
       </c>
       <c r="E1" s="33" t="s">
         <v>221</v>
@@ -9040,18 +9151,18 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="17.399999999999999">
+    <row r="2" spans="1:19" ht="17.5">
       <c r="A2" s="34" t="s">
-        <v>395</v>
+        <v>398</v>
       </c>
       <c r="B2" s="34" t="s">
-        <v>398</v>
+        <v>401</v>
       </c>
       <c r="C2" s="34" t="s">
         <v>289</v>
       </c>
       <c r="D2" s="34" t="s">
-        <v>409</v>
+        <v>414</v>
       </c>
       <c r="E2" s="35">
         <v>2</v>
@@ -9060,16 +9171,16 @@
         <v>351</v>
       </c>
       <c r="G2" s="36" t="s">
-        <v>418</v>
+        <v>404</v>
       </c>
       <c r="H2" s="32" t="s">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="I2" s="32" t="s">
         <v>84</v>
       </c>
       <c r="J2" s="32" t="s">
-        <v>399</v>
+        <v>402</v>
       </c>
       <c r="K2" s="33" t="s">
         <v>69</v>
@@ -9078,10 +9189,10 @@
         <v>8832</v>
       </c>
       <c r="M2" s="32" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="N2" s="32" t="s">
-        <v>400</v>
+        <v>403</v>
       </c>
       <c r="O2" s="37" t="s">
         <v>164</v>
@@ -9100,145 +9211,9 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
+  <phoneticPr fontId="22" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="G2" r:id="rId1" xr:uid="{887B28E3-50F7-4F52-8B2E-5EF4187C1BC4}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BAA440-EF09-47F4-83FC-456442901214}">
-  <dimension ref="A1:Q2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
-  <cols>
-    <col min="1" max="2" width="8.796875" style="33"/>
-    <col min="3" max="4" width="9.19921875" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.3984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.19921875" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="8.796875" style="33"/>
-    <col min="11" max="11" width="15.3984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="8.796875" style="33"/>
-    <col min="15" max="15" width="11.8984375" style="33" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.796875" style="33"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="33" t="s">
-        <v>402</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>149</v>
-      </c>
-      <c r="C1" s="33" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="33" t="s">
-        <v>393</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="33" t="s">
-        <v>60</v>
-      </c>
-      <c r="H1" s="33" t="s">
-        <v>221</v>
-      </c>
-      <c r="I1" s="33" t="s">
-        <v>410</v>
-      </c>
-      <c r="J1" s="33" t="s">
-        <v>411</v>
-      </c>
-      <c r="K1" s="33" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="33" t="s">
-        <v>64</v>
-      </c>
-      <c r="M1" s="33" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="33" t="s">
-        <v>215</v>
-      </c>
-      <c r="O1" s="33" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="33" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="33" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" ht="17.399999999999999">
-      <c r="A2" s="33" t="s">
-        <v>361</v>
-      </c>
-      <c r="B2" s="33" t="s">
-        <v>392</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>405</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>405</v>
-      </c>
-      <c r="E2" s="36" t="s">
-        <v>359</v>
-      </c>
-      <c r="F2" s="33" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="34" t="s">
-        <v>409</v>
-      </c>
-      <c r="H2" s="35">
-        <v>1</v>
-      </c>
-      <c r="I2" s="35">
-        <v>409776</v>
-      </c>
-      <c r="J2" s="35"/>
-      <c r="K2" s="32" t="s">
-        <v>403</v>
-      </c>
-      <c r="L2" s="32">
-        <v>9000</v>
-      </c>
-      <c r="M2" s="32" t="s">
-        <v>404</v>
-      </c>
-      <c r="N2" s="32" t="s">
-        <v>385</v>
-      </c>
-      <c r="O2" s="32" t="s">
-        <v>401</v>
-      </c>
-      <c r="P2" s="37" t="s">
-        <v>382</v>
-      </c>
-      <c r="Q2" s="33" t="s">
-        <v>413</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{40F20844-5117-47D6-BE5F-527AE99DDF41}"/>
-    <hyperlink ref="C2" r:id="rId2" display="chsqanew02@mailinator.com" xr:uid="{FD08E511-44B9-452F-B1A8-4D73F23D4B51}"/>
-    <hyperlink ref="D2" r:id="rId3" display="chsqanew02@mailinator.com" xr:uid="{6A3AE5FB-D30B-47A6-9922-6BB5284DC178}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9252,7 +9227,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -9324,6 +9299,138 @@
 </file>
 
 <file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BAA440-EF09-47F4-83FC-456442901214}">
+  <dimension ref="A1:P2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <cols>
+    <col min="1" max="2" width="8.83203125" style="33"/>
+    <col min="3" max="4" width="9.1640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.4140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.1640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="8.83203125" style="33"/>
+    <col min="11" max="11" width="15.4140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5" style="33" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="8.83203125" style="33"/>
+    <col min="15" max="15" width="11.9140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.83203125" style="33"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16">
+      <c r="A1" s="33" t="s">
+        <v>407</v>
+      </c>
+      <c r="B1" s="33" t="s">
+        <v>149</v>
+      </c>
+      <c r="C1" s="33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" s="33" t="s">
+        <v>396</v>
+      </c>
+      <c r="E1" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="H1" s="33" t="s">
+        <v>221</v>
+      </c>
+      <c r="I1" s="33" t="s">
+        <v>415</v>
+      </c>
+      <c r="J1" s="33" t="s">
+        <v>416</v>
+      </c>
+      <c r="K1" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="L1" s="33" t="s">
+        <v>64</v>
+      </c>
+      <c r="M1" s="33" t="s">
+        <v>44</v>
+      </c>
+      <c r="N1" s="33" t="s">
+        <v>215</v>
+      </c>
+      <c r="O1" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="P1" s="33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="17.5">
+      <c r="A2" s="33" t="s">
+        <v>362</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>395</v>
+      </c>
+      <c r="C2" s="36" t="s">
+        <v>410</v>
+      </c>
+      <c r="D2" s="36" t="s">
+        <v>410</v>
+      </c>
+      <c r="E2" s="36" t="s">
+        <v>359</v>
+      </c>
+      <c r="F2" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="34" t="s">
+        <v>414</v>
+      </c>
+      <c r="H2" s="35">
+        <v>1</v>
+      </c>
+      <c r="I2" s="35">
+        <v>409776</v>
+      </c>
+      <c r="J2" s="35">
+        <v>714131</v>
+      </c>
+      <c r="K2" s="32" t="s">
+        <v>408</v>
+      </c>
+      <c r="L2" s="32">
+        <v>9000</v>
+      </c>
+      <c r="M2" s="32" t="s">
+        <v>409</v>
+      </c>
+      <c r="N2" s="32" t="s">
+        <v>388</v>
+      </c>
+      <c r="O2" s="32" t="s">
+        <v>405</v>
+      </c>
+      <c r="P2" s="37" t="s">
+        <v>385</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1" xr:uid="{40F20844-5117-47D6-BE5F-527AE99DDF41}"/>
+    <hyperlink ref="C2" r:id="rId2" display="chsqanew02@mailinator.com" xr:uid="{FD08E511-44B9-452F-B1A8-4D73F23D4B51}"/>
+    <hyperlink ref="D2" r:id="rId3" display="chsqanew02@mailinator.com" xr:uid="{6A3AE5FB-D30B-47A6-9922-6BB5284DC178}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
@@ -9331,7 +9438,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -9376,7 +9483,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
   <dimension ref="A1:Q10"/>
   <sheetViews>
@@ -9384,7 +9491,7 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
     <col min="1" max="1" width="11" style="30"/>
   </cols>
@@ -9442,7 +9549,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.399999999999999">
+    <row r="2" spans="1:17" ht="17.5">
       <c r="A2" s="31" t="s">
         <v>285</v>
       </c>
@@ -9495,7 +9602,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.399999999999999">
+    <row r="3" spans="1:17" ht="17.5">
       <c r="A3" s="31" t="s">
         <v>342</v>
       </c>
@@ -9548,7 +9655,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.399999999999999">
+    <row r="4" spans="1:17" ht="17.5">
       <c r="A4" s="31" t="s">
         <v>343</v>
       </c>
@@ -9601,7 +9708,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.399999999999999">
+    <row r="5" spans="1:17" ht="17.5">
       <c r="A5" s="31" t="s">
         <v>344</v>
       </c>
@@ -9654,7 +9761,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17.399999999999999">
+    <row r="6" spans="1:17" ht="17.5">
       <c r="A6" s="31" t="s">
         <v>345</v>
       </c>
@@ -9707,7 +9814,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="17.399999999999999">
+    <row r="7" spans="1:17" ht="17.5">
       <c r="A7" s="31" t="s">
         <v>346</v>
       </c>
@@ -9760,7 +9867,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="17.399999999999999">
+    <row r="8" spans="1:17" ht="17.5">
       <c r="A8" s="31" t="s">
         <v>347</v>
       </c>
@@ -9813,7 +9920,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="17.399999999999999">
+    <row r="9" spans="1:17" ht="17.5">
       <c r="A9" s="31" t="s">
         <v>348</v>
       </c>
@@ -9866,7 +9973,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="17.399999999999999">
+    <row r="10" spans="1:17" ht="17.5">
       <c r="A10" s="31" t="s">
         <v>349</v>
       </c>
@@ -9929,7 +10036,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
   <dimension ref="A1:A13"/>
   <sheetViews>
@@ -9937,7 +10044,7 @@
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -10009,7 +10116,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AB2"/>
@@ -10018,13 +10125,13 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="35.3984375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.59765625" customWidth="1"/>
-    <col min="4" max="4" width="12.09765625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.3984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.4140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.58203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.58203125" customWidth="1"/>
+    <col min="4" max="4" width="12.08203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.4140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -10209,7 +10316,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -10217,7 +10324,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -10328,7 +10435,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -10336,7 +10443,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -10447,7 +10554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10455,7 +10562,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -10638,7 +10745,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10646,7 +10753,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -10829,7 +10936,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10837,7 +10944,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -11015,197 +11122,6 @@
   <hyperlinks>
     <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3A00-000000000000}"/>
     <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3A00-000001000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
-  <dimension ref="A1:AB2"/>
-  <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="U1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="X1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="1" t="s">
-        <v>206</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2333</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>238</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3B00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3B00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -11219,7 +11135,7 @@
       <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" t="s">
@@ -11253,7 +11169,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.8">
+    <row r="2" spans="1:10" ht="16.5">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -11291,6 +11207,197 @@
 </file>
 
 <file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2333</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3B00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3B00-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11298,7 +11405,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -11481,7 +11588,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11489,7 +11596,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -11672,7 +11779,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11680,7 +11787,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -11863,7 +11970,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -11871,7 +11978,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -12054,7 +12161,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12062,7 +12169,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -12245,7 +12352,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12253,7 +12360,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" s="18" t="s">
@@ -12436,7 +12543,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12444,7 +12551,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -12627,7 +12734,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12635,7 +12742,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -12818,7 +12925,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -12826,7 +12933,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -13005,197 +13112,6 @@
     <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4400-000000000000}"/>
     <hyperlink ref="H2" r:id="rId2" display="mailto:test01codem@gmail.com" xr:uid="{00000000-0004-0000-4400-000001000000}"/>
     <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-4400-000002000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
-  <dimension ref="A1:AB2"/>
-  <sheetViews>
-    <sheetView topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <sheetData>
-    <row r="1" spans="1:28">
-      <c r="A1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E1" t="s">
-        <v>27</v>
-      </c>
-      <c r="F1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G1" t="s">
-        <v>29</v>
-      </c>
-      <c r="H1" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J1" t="s">
-        <v>32</v>
-      </c>
-      <c r="K1" t="s">
-        <v>33</v>
-      </c>
-      <c r="L1" t="s">
-        <v>34</v>
-      </c>
-      <c r="M1" t="s">
-        <v>35</v>
-      </c>
-      <c r="N1" t="s">
-        <v>36</v>
-      </c>
-      <c r="O1" t="s">
-        <v>37</v>
-      </c>
-      <c r="P1" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>39</v>
-      </c>
-      <c r="R1" t="s">
-        <v>40</v>
-      </c>
-      <c r="S1" t="s">
-        <v>41</v>
-      </c>
-      <c r="T1" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="U1" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="V1" s="18" t="s">
-        <v>81</v>
-      </c>
-      <c r="W1" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="X1" t="s">
-        <v>45</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>49</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:28">
-      <c r="A2" s="1" t="s">
-        <v>208</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="E2" s="4">
-        <v>2333</v>
-      </c>
-      <c r="F2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>230</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="K2" t="s">
-        <v>158</v>
-      </c>
-      <c r="L2" t="s">
-        <v>70</v>
-      </c>
-      <c r="M2" t="s">
-        <v>53</v>
-      </c>
-      <c r="N2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="P2" t="s">
-        <v>158</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>70</v>
-      </c>
-      <c r="R2" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="T2" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="U2" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="V2" s="1" t="s">
-        <v>140</v>
-      </c>
-      <c r="W2" s="19" t="s">
-        <v>89</v>
-      </c>
-      <c r="X2" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="Z2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="AA2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="AB2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4500-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4500-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -13209,11 +13125,11 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultRowHeight="15.5"/>
   <cols>
-    <col min="1" max="1" width="15.69921875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.09765625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.08203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -13248,7 +13164,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="16.8">
+    <row r="2" spans="1:10" ht="16.5">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -13286,6 +13202,197 @@
 </file>
 
 <file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
+  <dimension ref="A1:AB2"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X2" sqref="X2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetData>
+    <row r="1" spans="1:28">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M1" t="s">
+        <v>35</v>
+      </c>
+      <c r="N1" t="s">
+        <v>36</v>
+      </c>
+      <c r="O1" t="s">
+        <v>37</v>
+      </c>
+      <c r="P1" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>39</v>
+      </c>
+      <c r="R1" t="s">
+        <v>40</v>
+      </c>
+      <c r="S1" t="s">
+        <v>41</v>
+      </c>
+      <c r="T1" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="U1" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="V1" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="W1" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="X1" t="s">
+        <v>45</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28">
+      <c r="A2" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="E2" s="4">
+        <v>2333</v>
+      </c>
+      <c r="F2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" t="s">
+        <v>43</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="K2" t="s">
+        <v>158</v>
+      </c>
+      <c r="L2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="P2" t="s">
+        <v>158</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>70</v>
+      </c>
+      <c r="R2" t="s">
+        <v>58</v>
+      </c>
+      <c r="S2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="T2" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="U2" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="W2" s="19" t="s">
+        <v>89</v>
+      </c>
+      <c r="X2" s="8" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AA2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4500-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4500-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -13293,7 +13400,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -13404,7 +13511,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -13412,7 +13519,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -13595,7 +13702,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -13603,7 +13710,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -13786,7 +13893,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -13794,7 +13901,7 @@
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -13905,7 +14012,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -13913,7 +14020,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -14097,7 +14204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -14105,7 +14212,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -14288,7 +14395,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4C00-000000000000}">
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -14296,7 +14403,7 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -14479,7 +14586,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4D00-000000000000}">
   <dimension ref="A1:N2"/>
   <sheetViews>
@@ -14487,7 +14594,7 @@
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -14533,7 +14640,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="20.399999999999999">
+    <row r="2" spans="1:14" ht="20">
       <c r="A2" s="20" t="s">
         <v>162</v>
       </c>
@@ -14585,7 +14692,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4E00-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -14593,7 +14700,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -14632,69 +14739,6 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-4E00-000000000000}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4F00-000000000000}">
-  <sheetPr codeName="Sheet15"/>
-  <dimension ref="A1:F2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
-  <cols>
-    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:6">
-      <c r="A1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" t="s">
-        <v>9</v>
-      </c>
-      <c r="F1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-4F00-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-4F00-000001000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -14708,9 +14752,9 @@
       <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <cols>
-    <col min="5" max="5" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -14783,6 +14827,69 @@
 </file>
 
 <file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4F00-000000000000}">
+  <sheetPr codeName="Sheet15"/>
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <cols>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-4F00-000000000000}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-4F00-000001000000}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5000-000000000000}">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:D2"/>
@@ -14791,7 +14898,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">

</xml_diff>

<commit_message>
Nikita's changes 24 Dec 2021
</commit_message>
<xml_diff>
--- a/TestData/PartyLite_Smokes_Data.xlsx
+++ b/TestData/PartyLite_Smokes_Data.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24527"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dell\Desktop\Automation_PL\relite-partylite-test-automation-462d32aa2b21\TestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E09C7E4-56BC-4BE1-84F2-DC491B2E254A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="51" activeTab="53" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="19425" windowHeight="10425" firstSheet="92" activeTab="95"/>
   </bookViews>
   <sheets>
     <sheet name="AddGuestDetails_PL" sheetId="17" r:id="rId1"/>
@@ -64,46 +58,51 @@
     <sheet name="PartyCreationConsAsHost_HA_PL" sheetId="8" r:id="rId49"/>
     <sheet name="VirtualSubmit_PL" sheetId="38" r:id="rId50"/>
     <sheet name="CustomerOrder_PL" sheetId="22" r:id="rId51"/>
-    <sheet name="Smoke_TestCase_2" sheetId="84" r:id="rId52"/>
-    <sheet name="Smoke_TestCase_3" sheetId="86" r:id="rId53"/>
-    <sheet name="Smoke_TestCase_4" sheetId="93" r:id="rId54"/>
-    <sheet name="Smoke_TestCase_6" sheetId="87" r:id="rId55"/>
-    <sheet name="Smoke_TestCase_7" sheetId="88" r:id="rId56"/>
-    <sheet name="Smoke_TestCase_8" sheetId="89" r:id="rId57"/>
-    <sheet name="Smoke_TestCase_10" sheetId="90" r:id="rId58"/>
-    <sheet name="Smoke_TestCase_11" sheetId="91" r:id="rId59"/>
-    <sheet name="Smoke_TestCase_12" sheetId="92" r:id="rId60"/>
-    <sheet name="MyAccount_Email_PL" sheetId="71" r:id="rId61"/>
-    <sheet name="GuestOrder_GC_PL" sheetId="23" r:id="rId62"/>
-    <sheet name="CategoryURL_PL" sheetId="49" r:id="rId63"/>
-    <sheet name="PaperOrderCreationDetails_PL" sheetId="7" r:id="rId64"/>
-    <sheet name="CollectivePT_PL" sheetId="39" r:id="rId65"/>
-    <sheet name="CollectivePT_FR_PL" sheetId="73" r:id="rId66"/>
-    <sheet name="ClassicPT_PL" sheetId="35" r:id="rId67"/>
-    <sheet name="ClassicPT_FR_PL" sheetId="72" r:id="rId68"/>
-    <sheet name="PO_DB1_PL" sheetId="55" r:id="rId69"/>
-    <sheet name="PO_DB2_PL" sheetId="56" r:id="rId70"/>
-    <sheet name="PO_DB3_PL" sheetId="57" r:id="rId71"/>
-    <sheet name="PO_DB4_PL" sheetId="58" r:id="rId72"/>
-    <sheet name="PO_DB5_PL" sheetId="59" r:id="rId73"/>
-    <sheet name="PO_DB6_PL" sheetId="60" r:id="rId74"/>
-    <sheet name="PO_DB7_PL" sheetId="61" r:id="rId75"/>
-    <sheet name="PO_DB8_PL" sheetId="62" r:id="rId76"/>
-    <sheet name="FYSPT_PL" sheetId="40" r:id="rId77"/>
-    <sheet name="FYSPT_FR_PL" sheetId="74" r:id="rId78"/>
-    <sheet name="ClassicPTRC_PL" sheetId="41" r:id="rId79"/>
-    <sheet name="ClassicPT_SC_PL" sheetId="42" r:id="rId80"/>
-    <sheet name="CollectivePT_SC_PL" sheetId="43" r:id="rId81"/>
-    <sheet name="FYSPT_SC_PL" sheetId="44" r:id="rId82"/>
-    <sheet name="ClassicPT_SH_PL" sheetId="45" r:id="rId83"/>
-    <sheet name="CollectivePT_SH_PL" sheetId="46" r:id="rId84"/>
-    <sheet name="FYSPT_SH_PL" sheetId="47" r:id="rId85"/>
-    <sheet name="ClassicPTCA_PL" sheetId="64" r:id="rId86"/>
-    <sheet name="FYSPTCA_PL" sheetId="66" r:id="rId87"/>
-    <sheet name="ShareParty_PL" sheetId="48" r:id="rId88"/>
-    <sheet name="PartyContactCreationNano_PL" sheetId="24" r:id="rId89"/>
-    <sheet name="PreventDupeAcctCreation_PL" sheetId="3" r:id="rId90"/>
-    <sheet name="SearchConsultant_PL" sheetId="4" r:id="rId91"/>
+    <sheet name="Smoke_TestCase_1" sheetId="94" r:id="rId52"/>
+    <sheet name="Smoke_TestCase_2" sheetId="84" r:id="rId53"/>
+    <sheet name="Smoke_TestCase_3" sheetId="86" r:id="rId54"/>
+    <sheet name="Smoke_TestCase_4" sheetId="93" r:id="rId55"/>
+    <sheet name="Smoke_TestCase_5" sheetId="95" r:id="rId56"/>
+    <sheet name="Smoke_TestCase_6" sheetId="87" r:id="rId57"/>
+    <sheet name="Smoke_TestCase_7" sheetId="88" r:id="rId58"/>
+    <sheet name="Smoke_TestCase_8" sheetId="89" r:id="rId59"/>
+    <sheet name="Smoke_TestCase_9" sheetId="96" r:id="rId60"/>
+    <sheet name="Smoke_TestCase_10" sheetId="90" r:id="rId61"/>
+    <sheet name="Regression_TC18" sheetId="97" r:id="rId62"/>
+    <sheet name="Smoke_TestCase_11" sheetId="91" r:id="rId63"/>
+    <sheet name="Smoke_TestCase_12" sheetId="92" r:id="rId64"/>
+    <sheet name="MyAccount_Email_PL" sheetId="71" r:id="rId65"/>
+    <sheet name="GuestOrder_GC_PL" sheetId="23" r:id="rId66"/>
+    <sheet name="CategoryURL_PL" sheetId="49" r:id="rId67"/>
+    <sheet name="PaperOrderCreationDetails_PL" sheetId="7" r:id="rId68"/>
+    <sheet name="CollectivePT_PL" sheetId="39" r:id="rId69"/>
+    <sheet name="CollectivePT_FR_PL" sheetId="73" r:id="rId70"/>
+    <sheet name="ClassicPT_PL" sheetId="35" r:id="rId71"/>
+    <sheet name="ClassicPT_FR_PL" sheetId="72" r:id="rId72"/>
+    <sheet name="PO_DB1_PL" sheetId="55" r:id="rId73"/>
+    <sheet name="PO_DB2_PL" sheetId="56" r:id="rId74"/>
+    <sheet name="PO_DB3_PL" sheetId="57" r:id="rId75"/>
+    <sheet name="PO_DB4_PL" sheetId="58" r:id="rId76"/>
+    <sheet name="PO_DB5_PL" sheetId="59" r:id="rId77"/>
+    <sheet name="PO_DB6_PL" sheetId="60" r:id="rId78"/>
+    <sheet name="PO_DB7_PL" sheetId="61" r:id="rId79"/>
+    <sheet name="PO_DB8_PL" sheetId="62" r:id="rId80"/>
+    <sheet name="FYSPT_PL" sheetId="40" r:id="rId81"/>
+    <sheet name="FYSPT_FR_PL" sheetId="74" r:id="rId82"/>
+    <sheet name="ClassicPTRC_PL" sheetId="41" r:id="rId83"/>
+    <sheet name="ClassicPT_SC_PL" sheetId="42" r:id="rId84"/>
+    <sheet name="CollectivePT_SC_PL" sheetId="43" r:id="rId85"/>
+    <sheet name="FYSPT_SC_PL" sheetId="44" r:id="rId86"/>
+    <sheet name="ClassicPT_SH_PL" sheetId="45" r:id="rId87"/>
+    <sheet name="CollectivePT_SH_PL" sheetId="46" r:id="rId88"/>
+    <sheet name="FYSPT_SH_PL" sheetId="47" r:id="rId89"/>
+    <sheet name="ClassicPTCA_PL" sheetId="64" r:id="rId90"/>
+    <sheet name="FYSPTCA_PL" sheetId="66" r:id="rId91"/>
+    <sheet name="ShareParty_PL" sheetId="48" r:id="rId92"/>
+    <sheet name="PartyContactCreationNano_PL" sheetId="24" r:id="rId93"/>
+    <sheet name="PreventDupeAcctCreation_PL" sheetId="3" r:id="rId94"/>
+    <sheet name="SearchConsultant_PL" sheetId="4" r:id="rId95"/>
+    <sheet name="GuestOrder_GC" sheetId="98" r:id="rId96"/>
   </sheets>
   <calcPr calcId="144525"/>
   <extLst>
@@ -115,7 +114,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3423" uniqueCount="421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3551" uniqueCount="448">
   <si>
     <t>Username</t>
   </si>
@@ -1378,15 +1377,124 @@
   </si>
   <si>
     <t>Yukon Territory</t>
+  </si>
+  <si>
+    <t>PSC 557 Box 3250</t>
+  </si>
+  <si>
+    <t>FPO</t>
+  </si>
+  <si>
+    <t>Armed Forces Pacific</t>
+  </si>
+  <si>
+    <t>96379</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>cphone</t>
+  </si>
+  <si>
+    <t>mphone</t>
+  </si>
+  <si>
+    <t>billaddress1</t>
+  </si>
+  <si>
+    <t>billcity</t>
+  </si>
+  <si>
+    <t>state1</t>
+  </si>
+  <si>
+    <t>billzipcode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Henbury Avenue </t>
+  </si>
+  <si>
+    <t>2848</t>
+  </si>
+  <si>
+    <t>Kandos</t>
+  </si>
+  <si>
+    <t>0212341234'</t>
+  </si>
+  <si>
+    <t>0401212345'</t>
+  </si>
+  <si>
+    <t>New South Wales</t>
+  </si>
+  <si>
+    <t>4680</t>
+  </si>
+  <si>
+    <t>01923 123456</t>
+  </si>
+  <si>
+    <t>Unit 1 51 Beach Street</t>
+  </si>
+  <si>
+    <t>7018</t>
+  </si>
+  <si>
+    <t>Bellerive</t>
+  </si>
+  <si>
+    <t>Tasmania</t>
+  </si>
+  <si>
+    <t>giftnum</t>
+  </si>
+  <si>
+    <t>giftpin</t>
+  </si>
+  <si>
+    <t>803509</t>
+  </si>
+  <si>
+    <t>1191810</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="32">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1536,6 +1644,34 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF454545"/>
+      <name val="Helvetica Neue"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF202124"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Docs-Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1556,56 +1692,66 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="1" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" quotePrefix="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -1668,7 +1814,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -1720,7 +1866,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -1914,14 +2060,14 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet17"/>
   <dimension ref="A1:Z2"/>
   <sheetViews>
@@ -1929,10 +2075,10 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="35.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -2097,24 +2243,24 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="5" max="5" width="12.4140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2187,14 +2333,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -2370,21 +2516,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-0900-000000000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:F3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -2406,7 +2552,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="20">
+    <row r="2" spans="1:6" ht="20.25">
       <c r="A2" s="12" t="s">
         <v>110</v>
       </c>
@@ -2452,14 +2598,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -2515,21 +2661,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0B00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -2591,21 +2737,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0C00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -2655,21 +2801,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0D00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -2707,21 +2853,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0E00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -2759,21 +2905,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-0F00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
@@ -2847,21 +2993,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-1000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -2953,21 +3099,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-1100-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -3037,7 +3183,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="17.5">
+    <row r="5" spans="1:5" ht="18">
       <c r="A5" s="11" t="s">
         <v>105</v>
       </c>
@@ -3054,7 +3200,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="17.5">
+    <row r="6" spans="1:5" ht="18">
       <c r="A6" s="11" t="s">
         <v>300</v>
       </c>
@@ -3077,14 +3223,14 @@
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -3128,22 +3274,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com" xr:uid="{00000000-0004-0000-1200-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-1200-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -3187,22 +3333,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com" xr:uid="{00000000-0004-0000-1300-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-1300-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -3282,15 +3428,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com" xr:uid="{00000000-0004-0000-1400-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-1400-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -3298,11 +3444,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="35.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.58203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.08203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -3371,22 +3517,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" display="Codemtest@mailinator.com" xr:uid="{00000000-0004-0000-1500-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-1500-000001000000}"/>
+    <hyperlink ref="E2" r:id="rId1" display="Codemtest@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:18">
       <c r="A1" t="s">
@@ -3444,7 +3590,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.5">
+    <row r="2" spans="1:18" ht="18">
       <c r="A2" t="s">
         <v>217</v>
       </c>
@@ -3502,22 +3648,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="codemdemo_testconsultant20@mailinator.com" xr:uid="{00000000-0004-0000-1600-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" display="codemdemo_testconsultant20@mailinator.com" xr:uid="{00000000-0004-0000-1600-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1" display="codemdemo_testconsultant20@mailinator.com"/>
+    <hyperlink ref="D2" r:id="rId2" display="codemdemo_testconsultant20@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -3693,22 +3839,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-1700-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-1700-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -3752,22 +3898,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-1800-000000000000}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{00000000-0004-0000-1800-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -3781,14 +3927,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-1900-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -3796,10 +3942,10 @@
       <selection activeCell="F7" sqref="F6:F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.08203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="25.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -3844,8 +3990,8 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="joanne@mailintor.com" xr:uid="{00000000-0004-0000-1A00-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" display="joanne@mailintor.com" xr:uid="{00000000-0004-0000-1A00-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1" display="joanne@mailintor.com"/>
+    <hyperlink ref="D2" r:id="rId2" display="joanne@mailintor.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -3853,7 +3999,7 @@
 </file>
 
 <file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -3861,10 +4007,10 @@
       <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="23.9140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.9140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -3920,7 +4066,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.5">
+    <row r="2" spans="1:17" ht="18">
       <c r="A2" s="1" t="s">
         <v>86</v>
       </c>
@@ -3975,22 +4121,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-1B00-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-1B00-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -4042,7 +4188,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17.5">
+    <row r="2" spans="1:16" ht="18">
       <c r="A2" s="16" t="s">
         <v>97</v>
       </c>
@@ -4094,14 +4240,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="qacwscategory_guestorder@mailinator.com" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="qacwscategory_guestorder@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -4109,10 +4255,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="35.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -4123,7 +4269,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="20">
+    <row r="2" spans="1:2" ht="20.25">
       <c r="A2" s="20" t="s">
         <v>162</v>
       </c>
@@ -4137,7 +4283,7 @@
 </file>
 
 <file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet5"/>
   <dimension ref="A1:Q2"/>
   <sheetViews>
@@ -4145,7 +4291,7 @@
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -4255,15 +4401,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com" xr:uid="{00000000-0004-0000-1D00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-1D00-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:R2"/>
   <sheetViews>
@@ -4271,7 +4417,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="28" customWidth="1"/>
   </cols>
@@ -4332,7 +4478,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.5">
+    <row r="2" spans="1:18" ht="18">
       <c r="A2" s="5" t="s">
         <v>332</v>
       </c>
@@ -4390,21 +4536,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-1E00-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId1" display="qacws_guestorderuk@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-1F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -4428,17 +4574,17 @@
 </file>
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E79"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="24.08203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.58203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="24.125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
@@ -5262,14 +5408,14 @@
 </file>
 
 <file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -5294,14 +5440,14 @@
 </file>
 
 <file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -5356,7 +5502,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.5">
+    <row r="2" spans="1:17" ht="18">
       <c r="A2" s="5" t="s">
         <v>287</v>
       </c>
@@ -5409,7 +5555,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.5">
+    <row r="3" spans="1:17" ht="18">
       <c r="A3" s="5" t="s">
         <v>288</v>
       </c>
@@ -5462,7 +5608,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.5">
+    <row r="4" spans="1:17" ht="18">
       <c r="A4" s="5" t="s">
         <v>289</v>
       </c>
@@ -5515,7 +5661,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.5">
+    <row r="5" spans="1:17" ht="18">
       <c r="A5" s="5" t="s">
         <v>285</v>
       </c>
@@ -5568,7 +5714,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="20">
+    <row r="6" spans="1:17" ht="20.25">
       <c r="A6" s="13" t="s">
         <v>293</v>
       </c>
@@ -5623,27 +5769,27 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-2200-000000000000}"/>
-    <hyperlink ref="C3" r:id="rId2" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-2200-000001000000}"/>
-    <hyperlink ref="C4" r:id="rId3" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-2200-000002000000}"/>
-    <hyperlink ref="C5" r:id="rId4" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-2200-000003000000}"/>
-    <hyperlink ref="C6" r:id="rId5" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-2200-000004000000}"/>
+    <hyperlink ref="C2" r:id="rId1" display="qacws_guestorderuk@mailinator.com"/>
+    <hyperlink ref="C3" r:id="rId2" display="qacws_guestorderuk@mailinator.com"/>
+    <hyperlink ref="C4" r:id="rId3" display="qacws_guestorderuk@mailinator.com"/>
+    <hyperlink ref="C5" r:id="rId4" display="qacws_guestorderuk@mailinator.com"/>
+    <hyperlink ref="C6" r:id="rId5" display="qacws_guestorderuk@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
@@ -5702,7 +5848,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:18" ht="17.5">
+    <row r="2" spans="1:18" ht="18">
       <c r="A2" s="5" t="s">
         <v>289</v>
       </c>
@@ -5758,7 +5904,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="17.5">
+    <row r="3" spans="1:18" ht="18">
       <c r="A3" s="5" t="s">
         <v>288</v>
       </c>
@@ -5814,7 +5960,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="17.5">
+    <row r="4" spans="1:18" ht="18">
       <c r="A4" s="5" t="s">
         <v>289</v>
       </c>
@@ -5870,7 +6016,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:18" ht="17.5">
+    <row r="5" spans="1:18" ht="18">
       <c r="A5" s="5" t="s">
         <v>285</v>
       </c>
@@ -5926,7 +6072,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:18" ht="20">
+    <row r="6" spans="1:18" ht="20.25">
       <c r="A6" s="13" t="s">
         <v>293</v>
       </c>
@@ -5984,25 +6130,25 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-2300-000000000000}"/>
-    <hyperlink ref="D3" r:id="rId2" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-2300-000001000000}"/>
-    <hyperlink ref="D4" r:id="rId3" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-2300-000002000000}"/>
-    <hyperlink ref="D5" r:id="rId4" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-2300-000003000000}"/>
-    <hyperlink ref="D6" r:id="rId5" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-2300-000004000000}"/>
+    <hyperlink ref="D2" r:id="rId1" display="qacws_guestorderuk@mailinator.com"/>
+    <hyperlink ref="D3" r:id="rId2" display="qacws_guestorderuk@mailinator.com"/>
+    <hyperlink ref="D4" r:id="rId3" display="qacws_guestorderuk@mailinator.com"/>
+    <hyperlink ref="D5" r:id="rId4" display="qacws_guestorderuk@mailinator.com"/>
+    <hyperlink ref="D6" r:id="rId5" display="qacws_guestorderuk@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -6349,14 +6495,14 @@
 </file>
 
 <file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:12">
       <c r="A1" t="s">
@@ -6778,42 +6924,42 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-2500-000000000000}"/>
-    <hyperlink ref="C3:C11" r:id="rId2" display="testconsultant3@mailinator.com" xr:uid="{00000000-0004-0000-2500-000001000000}"/>
-    <hyperlink ref="C3" r:id="rId3" xr:uid="{00000000-0004-0000-2500-000002000000}"/>
-    <hyperlink ref="C4" r:id="rId4" xr:uid="{00000000-0004-0000-2500-000003000000}"/>
-    <hyperlink ref="C5" r:id="rId5" xr:uid="{00000000-0004-0000-2500-000004000000}"/>
-    <hyperlink ref="C6" r:id="rId6" xr:uid="{00000000-0004-0000-2500-000005000000}"/>
-    <hyperlink ref="C7" r:id="rId7" xr:uid="{00000000-0004-0000-2500-000006000000}"/>
-    <hyperlink ref="C8" r:id="rId8" xr:uid="{00000000-0004-0000-2500-000007000000}"/>
-    <hyperlink ref="C9" r:id="rId9" xr:uid="{00000000-0004-0000-2500-000008000000}"/>
-    <hyperlink ref="C10" r:id="rId10" xr:uid="{00000000-0004-0000-2500-000009000000}"/>
-    <hyperlink ref="C11" r:id="rId11" xr:uid="{00000000-0004-0000-2500-00000A000000}"/>
-    <hyperlink ref="D2" r:id="rId12" xr:uid="{00000000-0004-0000-2500-00000B000000}"/>
-    <hyperlink ref="D3:D11" r:id="rId13" display="testconsultant3@mailinator.com" xr:uid="{00000000-0004-0000-2500-00000C000000}"/>
-    <hyperlink ref="D3" r:id="rId14" xr:uid="{00000000-0004-0000-2500-00000D000000}"/>
-    <hyperlink ref="D4" r:id="rId15" xr:uid="{00000000-0004-0000-2500-00000E000000}"/>
-    <hyperlink ref="D5" r:id="rId16" xr:uid="{00000000-0004-0000-2500-00000F000000}"/>
-    <hyperlink ref="D6" r:id="rId17" xr:uid="{00000000-0004-0000-2500-000010000000}"/>
-    <hyperlink ref="D7" r:id="rId18" xr:uid="{00000000-0004-0000-2500-000011000000}"/>
-    <hyperlink ref="D8" r:id="rId19" xr:uid="{00000000-0004-0000-2500-000012000000}"/>
-    <hyperlink ref="D9" r:id="rId20" xr:uid="{00000000-0004-0000-2500-000013000000}"/>
-    <hyperlink ref="D10" r:id="rId21" xr:uid="{00000000-0004-0000-2500-000014000000}"/>
-    <hyperlink ref="D11" r:id="rId22" xr:uid="{00000000-0004-0000-2500-000015000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="C3:C11" r:id="rId2" display="testconsultant3@mailinator.com"/>
+    <hyperlink ref="C3" r:id="rId3"/>
+    <hyperlink ref="C4" r:id="rId4"/>
+    <hyperlink ref="C5" r:id="rId5"/>
+    <hyperlink ref="C6" r:id="rId6"/>
+    <hyperlink ref="C7" r:id="rId7"/>
+    <hyperlink ref="C8" r:id="rId8"/>
+    <hyperlink ref="C9" r:id="rId9"/>
+    <hyperlink ref="C10" r:id="rId10"/>
+    <hyperlink ref="C11" r:id="rId11"/>
+    <hyperlink ref="D2" r:id="rId12"/>
+    <hyperlink ref="D3:D11" r:id="rId13" display="testconsultant3@mailinator.com"/>
+    <hyperlink ref="D3" r:id="rId14"/>
+    <hyperlink ref="D4" r:id="rId15"/>
+    <hyperlink ref="D5" r:id="rId16"/>
+    <hyperlink ref="D6" r:id="rId17"/>
+    <hyperlink ref="D7" r:id="rId18"/>
+    <hyperlink ref="D8" r:id="rId19"/>
+    <hyperlink ref="D9" r:id="rId20"/>
+    <hyperlink ref="D10" r:id="rId21"/>
+    <hyperlink ref="D11" r:id="rId22"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -6865,7 +7011,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17.5">
+    <row r="2" spans="1:16" ht="18">
       <c r="A2" s="16" t="s">
         <v>95</v>
       </c>
@@ -6917,14 +7063,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="qacwscategory_guestorder@mailinator.com" xr:uid="{00000000-0004-0000-0300-000000000000}"/>
+    <hyperlink ref="B2" r:id="rId1" display="qacwscategory_guestorder@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:B2"/>
   <sheetViews>
@@ -6932,7 +7078,7 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
@@ -6952,22 +7098,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" display="anushanand55@gmail.com" xr:uid="{00000000-0004-0000-2600-000000000000}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{00000000-0004-0000-2600-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId1" display="anushanand55@gmail.com"/>
+    <hyperlink ref="B2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2700-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
@@ -7016,7 +7162,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17.5">
+    <row r="2" spans="1:15" ht="18">
       <c r="A2" t="s">
         <v>14</v>
       </c>
@@ -7069,14 +7215,14 @@
 </file>
 
 <file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2800-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -7131,7 +7277,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.5">
+    <row r="2" spans="1:17" ht="18">
       <c r="A2" t="s">
         <v>194</v>
       </c>
@@ -7190,14 +7336,14 @@
 </file>
 
 <file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2900-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:13">
       <c r="A1" t="s">
@@ -7240,7 +7386,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="17.5">
+    <row r="2" spans="1:13" ht="18">
       <c r="A2" t="s">
         <v>23</v>
       </c>
@@ -7287,7 +7433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2A00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet8"/>
   <dimension ref="A1:S2"/>
   <sheetViews>
@@ -7295,10 +7441,10 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="9" max="9" width="11.08203125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="16.58203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="16.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -7421,14 +7567,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-2A00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2B00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet9"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -7436,9 +7582,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="6" max="6" width="20.58203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -7483,15 +7629,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com" xr:uid="{00000000-0004-0000-2B00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-2B00-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2C00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet10"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -7499,7 +7645,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
@@ -7543,15 +7689,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com" xr:uid="{00000000-0004-0000-2C00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-2C00-000001000000}"/>
+    <hyperlink ref="F2" r:id="rId1" display="Codemtest@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2D00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet11"/>
   <dimension ref="A1:P2"/>
   <sheetViews>
@@ -7559,7 +7705,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -7663,14 +7809,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-2D00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2E00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet12"/>
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -7678,7 +7824,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -7716,14 +7862,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-2E00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-2F00-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet13"/>
   <dimension ref="A1:E2"/>
   <sheetViews>
@@ -7731,7 +7877,7 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -7769,21 +7915,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-2F00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
@@ -7838,7 +7984,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.5">
+    <row r="2" spans="1:17" ht="18">
       <c r="A2" s="5" t="s">
         <v>253</v>
       </c>
@@ -7893,7 +8039,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="C2" r:id="rId1" display="qacws_guestorderuk@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId2"/>
@@ -7901,14 +8047,14 @@
 </file>
 
 <file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:8">
       <c r="A1" t="s">
@@ -7964,23 +8110,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-3000-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -8036,7 +8182,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.5">
+    <row r="2" spans="1:17" ht="18">
       <c r="A2" s="1" t="s">
         <v>353</v>
       </c>
@@ -8103,29 +8249,111 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{7BD1B739-4E76-453B-A163-373C059AFEAA}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00557CE2-344E-4748-8050-502ACD386C65}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>421</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>424</v>
+      </c>
+      <c r="D2" t="s">
+        <v>422</v>
+      </c>
+      <c r="E2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F2" t="s">
+        <v>423</v>
+      </c>
+      <c r="G2" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>425</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:Q2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.4140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.4140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8182,7 +8410,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.5">
+    <row r="2" spans="1:17" ht="18">
       <c r="A2" s="1" t="s">
         <v>360</v>
       </c>
@@ -8237,15 +8465,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{F0A9B555-A9E5-4569-8C63-F3EB03DD41FA}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{8F42B2BA-72E7-4561-A341-C3A2E2747D66}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5AF99577-3E21-4F91-8A0E-F977C7E7598B}">
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -8255,13 +8483,13 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="18.6640625" customWidth="1"/>
-    <col min="6" max="6" width="15.4140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="18.625" customWidth="1"/>
+    <col min="6" max="6" width="15.375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="11.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.9140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
@@ -8317,7 +8545,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.5">
+    <row r="2" spans="1:17" ht="18">
       <c r="A2" s="5" t="s">
         <v>354</v>
       </c>
@@ -8372,34 +8600,34 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{209DDE12-9F8E-43EB-ADC3-96C4571EC58A}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34C2D9A-3197-4887-BB87-C55FC188EBDB}">
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.4140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="11.9140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.58203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="21.4140625" style="41" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.375" style="41" customWidth="1"/>
+    <col min="8" max="8" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="7.75" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8472,8 +8700,128 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{377BF7CB-F633-49F4-8D49-EB8446EAC16C}">
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:O2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.75" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:15" s="30" customFormat="1">
+      <c r="A1" s="30" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="30" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" s="30" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" s="30" t="s">
+        <v>426</v>
+      </c>
+      <c r="F1" s="30" t="s">
+        <v>427</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>215</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>428</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>429</v>
+      </c>
+      <c r="J1" s="44" t="s">
+        <v>430</v>
+      </c>
+      <c r="K1" s="44" t="s">
+        <v>431</v>
+      </c>
+      <c r="L1" s="30" t="s">
+        <v>47</v>
+      </c>
+      <c r="M1" s="30" t="s">
+        <v>48</v>
+      </c>
+      <c r="N1" s="30" t="s">
+        <v>49</v>
+      </c>
+      <c r="O1" s="30" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>432</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>433</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="E2" s="45" t="s">
+        <v>435</v>
+      </c>
+      <c r="F2" s="46" t="s">
+        <v>436</v>
+      </c>
+      <c r="G2" s="47" t="s">
+        <v>437</v>
+      </c>
+      <c r="H2" s="44" t="s">
+        <v>372</v>
+      </c>
+      <c r="I2" s="44" t="s">
+        <v>373</v>
+      </c>
+      <c r="J2" s="47" t="s">
+        <v>374</v>
+      </c>
+      <c r="K2" s="48" t="s">
+        <v>438</v>
+      </c>
+      <c r="L2" s="49" t="s">
+        <v>214</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -8483,16 +8831,16 @@
       <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="2" max="2" width="4.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="4.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.58203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.4140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.9140625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10.9140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -8560,7 +8908,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="2" spans="1:21" ht="17.5">
+    <row r="2" spans="1:21" ht="18">
       <c r="A2" s="5" t="s">
         <v>354</v>
       </c>
@@ -8627,15 +8975,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{807A3D09-D1F7-43E4-8612-AABB53C9F8DD}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E84195DF-01B2-4D45-8E2B-90A4FB63FF02}">
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -8645,21 +8993,21 @@
       <selection activeCell="I2" sqref="I2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="8.83203125" style="33"/>
-    <col min="2" max="2" width="4.1640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.875" style="33"/>
+    <col min="2" max="2" width="4.125" style="33" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" style="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.58203125" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.4140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.83203125" style="33"/>
-    <col min="9" max="9" width="7.33203125" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.33203125" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.33203125" style="33" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.625" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.875" style="33"/>
+    <col min="9" max="9" width="7.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.375" style="33" customWidth="1"/>
+    <col min="12" max="12" width="18.375" style="33" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="33"/>
+    <col min="14" max="16384" width="8.875" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -8721,7 +9069,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="17.5">
+    <row r="2" spans="1:19" ht="18">
       <c r="A2" s="34" t="s">
         <v>354</v>
       </c>
@@ -8782,15 +9130,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{318A39AA-72BA-4A66-A3C8-5DCE254FC2E2}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{622CFA83-E905-4467-BCFD-8E7E2CF53AA9}">
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -8800,14 +9148,14 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="25.58203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.4140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="25.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.4140625" customWidth="1"/>
-    <col min="5" max="5" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.4140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="20.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.375" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -8870,7 +9218,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="17.5">
+    <row r="2" spans="1:19" ht="18">
       <c r="A2" s="1" t="s">
         <v>389</v>
       </c>
@@ -8931,16 +9279,186 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{83A341BD-A415-4EC1-9C7D-53D27E82D078}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{A0B128BF-5C69-492F-9E25-60EC8B6D8510}"/>
-    <hyperlink ref="C2" r:id="rId3" display="test_smoke0410@mailinator.com" xr:uid="{4DCE5C32-E792-4E94-959E-DB85BFA4F127}"/>
+    <hyperlink ref="B2" r:id="rId1"/>
+    <hyperlink ref="A2" r:id="rId2"/>
+    <hyperlink ref="C2" r:id="rId3" display="test_smoke0410@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9962DFF2-70D3-42DF-A705-EB69D22B5F41}">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>324</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>325</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>337</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>335</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>336</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>439</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>326</v>
+      </c>
+      <c r="G2" s="50" t="s">
+        <v>118</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor rgb="FFFFFF00"/>
   </sheetPr>
@@ -8950,19 +9468,19 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="33"/>
-    <col min="3" max="4" width="9.33203125" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.4140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="8.83203125" style="33"/>
-    <col min="9" max="9" width="15.4140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.875" style="33"/>
+    <col min="3" max="4" width="9.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.125" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="8.875" style="33"/>
+    <col min="9" max="9" width="15.375" style="33" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="12" width="8.83203125" style="33"/>
-    <col min="13" max="13" width="11.9140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="11.9140625" style="33" customWidth="1"/>
-    <col min="15" max="16384" width="8.83203125" style="33"/>
+    <col min="11" max="12" width="8.875" style="33"/>
+    <col min="13" max="13" width="11.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.875" style="33" customWidth="1"/>
+    <col min="15" max="16384" width="8.875" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
@@ -9012,7 +9530,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="17.5">
+    <row r="2" spans="1:15" ht="18">
       <c r="A2" s="33" t="s">
         <v>362</v>
       </c>
@@ -9061,35 +9579,117 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{83C30567-2619-416A-8A3B-3616C36A4346}"/>
-    <hyperlink ref="C2" r:id="rId2" display="uksqanew10@mailinator.com" xr:uid="{1B909638-F0A6-424A-A3B0-75B23D4BBC00}"/>
-    <hyperlink ref="D2" r:id="rId3" display="uksqanew10@mailinator.com" xr:uid="{DCFC5EAD-59D0-4AF8-B14D-9C3562C8FA05}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2" display="uksqanew10@mailinator.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="uksqanew10@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BABC2C4D-D525-4D71-9D7D-8F9EC67442AC}">
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FFFFFF00"/>
+  </sheetPr>
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>440</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>441</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>442</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="G2" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="K17" sqref="K17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="4" width="8.83203125" style="33"/>
-    <col min="5" max="5" width="4.1640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" style="33" customWidth="1"/>
-    <col min="7" max="7" width="18.6640625" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="8.875" style="33"/>
+    <col min="5" max="5" width="4.125" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.625" style="33" customWidth="1"/>
+    <col min="7" max="7" width="18.625" style="33" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="9.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.58203125" style="33" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.4140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.83203125" style="33"/>
+    <col min="9" max="9" width="8.625" style="33" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.875" style="33"/>
     <col min="12" max="12" width="11.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.33203125" style="33" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="8.83203125" style="33"/>
+    <col min="13" max="13" width="12.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="8.875" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19">
@@ -9151,7 +9751,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:19" ht="17.5">
+    <row r="2" spans="1:19" ht="18">
       <c r="A2" s="34" t="s">
         <v>398</v>
       </c>
@@ -9211,113 +9811,34 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="22" type="noConversion"/>
+  <phoneticPr fontId="26" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="G2" r:id="rId1" xr:uid="{887B28E3-50F7-4F52-8B2E-5EF4187C1BC4}"/>
+    <hyperlink ref="G2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>324</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>325</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>326</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87BAA440-EF09-47F4-83FC-456442901214}">
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83203125" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="8.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="8.83203125" style="33"/>
-    <col min="3" max="4" width="9.1640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.4140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="20.1640625" style="33" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="8.83203125" style="33"/>
-    <col min="11" max="11" width="15.4140625" style="33" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="8.875" style="33"/>
+    <col min="3" max="4" width="9.125" style="33" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.375" style="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.125" style="33" bestFit="1" customWidth="1"/>
+    <col min="7" max="10" width="8.875" style="33"/>
+    <col min="11" max="11" width="15.375" style="33" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11.5" style="33" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="8.83203125" style="33"/>
-    <col min="15" max="15" width="11.9140625" style="33" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="8.83203125" style="33"/>
+    <col min="13" max="14" width="8.875" style="33"/>
+    <col min="15" max="15" width="11.875" style="33" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="8.875" style="33"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -9370,7 +9891,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:16" ht="17.5">
+    <row r="2" spans="1:16" ht="18">
       <c r="A2" s="33" t="s">
         <v>362</v>
       </c>
@@ -9422,23 +9943,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E2" r:id="rId1" xr:uid="{40F20844-5117-47D6-BE5F-527AE99DDF41}"/>
-    <hyperlink ref="C2" r:id="rId2" display="chsqanew02@mailinator.com" xr:uid="{FD08E511-44B9-452F-B1A8-4D73F23D4B51}"/>
-    <hyperlink ref="D2" r:id="rId3" display="chsqanew02@mailinator.com" xr:uid="{6A3AE5FB-D30B-47A6-9922-6BB5284DC178}"/>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="C2" r:id="rId2" display="chsqanew02@mailinator.com"/>
+    <hyperlink ref="D2" r:id="rId3" display="chsqanew02@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3200-000000000000}">
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
@@ -9475,23 +9996,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-3200-000000000000}"/>
-    <hyperlink ref="A3" r:id="rId2" display="testconsultant3@mailinator.com" xr:uid="{00000000-0004-0000-3200-000001000000}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{00000000-0004-0000-3200-000002000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="A3" r:id="rId2" display="testconsultant3@mailinator.com"/>
+    <hyperlink ref="A3" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3300-000000000000}">
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Q10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="11" style="30"/>
   </cols>
@@ -9549,7 +10070,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:17" ht="17.5">
+    <row r="2" spans="1:17" ht="18">
       <c r="A2" s="31" t="s">
         <v>285</v>
       </c>
@@ -9602,7 +10123,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:17" ht="17.5">
+    <row r="3" spans="1:17" ht="18">
       <c r="A3" s="31" t="s">
         <v>342</v>
       </c>
@@ -9655,7 +10176,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="17.5">
+    <row r="4" spans="1:17" ht="18">
       <c r="A4" s="31" t="s">
         <v>343</v>
       </c>
@@ -9708,7 +10229,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:17" ht="17.5">
+    <row r="5" spans="1:17" ht="18">
       <c r="A5" s="31" t="s">
         <v>344</v>
       </c>
@@ -9761,7 +10282,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:17" ht="17.5">
+    <row r="6" spans="1:17" ht="18">
       <c r="A6" s="31" t="s">
         <v>345</v>
       </c>
@@ -9814,7 +10335,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="7" spans="1:17" ht="17.5">
+    <row r="7" spans="1:17" ht="18">
       <c r="A7" s="31" t="s">
         <v>346</v>
       </c>
@@ -9867,7 +10388,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="8" spans="1:17" ht="17.5">
+    <row r="8" spans="1:17" ht="18">
       <c r="A8" s="31" t="s">
         <v>347</v>
       </c>
@@ -9920,7 +10441,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:17" ht="17.5">
+    <row r="9" spans="1:17" ht="18">
       <c r="A9" s="31" t="s">
         <v>348</v>
       </c>
@@ -9973,7 +10494,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="10" spans="1:17" ht="17.5">
+    <row r="10" spans="1:17" ht="18">
       <c r="A10" s="31" t="s">
         <v>349</v>
       </c>
@@ -10028,23 +10549,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-3300-000000000000}"/>
-    <hyperlink ref="D3:D10" r:id="rId2" display="qacws_guestorderuk@mailinator.com" xr:uid="{00000000-0004-0000-3300-000001000000}"/>
+    <hyperlink ref="D2" r:id="rId1" display="qacws_guestorderuk@mailinator.com"/>
+    <hyperlink ref="D3:D10" r:id="rId2" display="qacws_guestorderuk@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3400-000000000000}">
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
@@ -10116,8 +10637,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3500-000000000000}">
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet14"/>
   <dimension ref="A1:AB2"/>
   <sheetViews>
@@ -10125,13 +10646,13 @@
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="35.4140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.58203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.58203125" customWidth="1"/>
-    <col min="4" max="4" width="12.08203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.4140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.625" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -10308,23 +10829,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3500-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3500-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3600-000000000000}">
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -10428,22 +10949,101 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3600-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3600-000001000000}"/>
+    <hyperlink ref="J2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3700-000000000000}">
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.5">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -10547,22 +11147,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3700-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3700-000001000000}"/>
+    <hyperlink ref="J2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3800-000000000000}">
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -10738,22 +11338,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3800-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3800-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3900-000000000000}">
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -10929,22 +11529,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3900-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3900-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3A00-000000000000}">
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -11120,101 +11720,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3A00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3A00-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>261</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3B00-000000000000}">
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -11390,22 +11911,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3B00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3B00-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3C00-000000000000}">
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -11581,22 +12102,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3C00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3C00-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3D00-000000000000}">
+<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -11772,22 +12293,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3D00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3D00-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3E00-000000000000}">
+<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -11963,22 +12484,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3E00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3E00-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-3F00-000000000000}">
+<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -12154,22 +12675,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-3F00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-3F00-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4000-000000000000}">
+<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -12345,22 +12866,106 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4000-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4000-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet76.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4100-000000000000}">
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <cols>
+    <col min="1" max="1" width="15.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="16.5">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>260</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>261</v>
+      </c>
+      <c r="E2" s="27" t="s">
+        <v>263</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>262</v>
+      </c>
+      <c r="G2" s="28" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" s="18" t="s">
@@ -12536,22 +13141,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-4100-000000000000}"/>
-    <hyperlink ref="V2" r:id="rId2" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4100-000001000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
+    <hyperlink ref="V2" r:id="rId2" display="mailto:guestPrivy@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet77.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4200-000000000000}">
+<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -12727,22 +13332,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4200-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4200-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet78.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4300-000000000000}">
+<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -12918,22 +13523,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4300-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4300-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet79.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4400-000000000000}">
+<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -13109,107 +13714,23 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4400-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" display="mailto:test01codem@gmail.com" xr:uid="{00000000-0004-0000-4400-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-4400-000002000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="H2" r:id="rId2" display="mailto:test01codem@gmail.com"/>
+    <hyperlink ref="A2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CCF2C1E-628B-4BC7-AE6E-3B1E5B8F517C}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5"/>
-  <cols>
-    <col min="1" max="1" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.08203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" ht="16.5">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="27" t="s">
-        <v>259</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>260</v>
-      </c>
-      <c r="D2" s="27" t="s">
-        <v>261</v>
-      </c>
-      <c r="E2" s="27" t="s">
-        <v>263</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>262</v>
-      </c>
-      <c r="G2" s="28" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet80.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4500-000000000000}">
+<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -13385,22 +13906,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4500-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4500-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet81.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4600-000000000000}">
+<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -13504,22 +14025,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4600-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4600-000001000000}"/>
+    <hyperlink ref="J2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet82.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4700-000000000000}">
+<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -13695,22 +14216,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4700-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4700-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet83.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4800-000000000000}">
+<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -13886,22 +14407,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4800-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4800-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet84.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4900-000000000000}">
+<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:16">
       <c r="A1" t="s">
@@ -14005,22 +14526,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4900-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4900-000001000000}"/>
+    <hyperlink ref="J2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet85.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4A00-000000000000}">
+<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -14196,23 +14717,105 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4A00-000000000000}"/>
-    <hyperlink ref="H2" r:id="rId2" display="codemdemo_classic@mailinator.com" xr:uid="{00000000-0004-0000-4A00-000001000000}"/>
-    <hyperlink ref="A2" r:id="rId3" xr:uid="{00000000-0004-0000-4A00-000002000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="H2" r:id="rId2" display="codemdemo_classic@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet86.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4B00-000000000000}">
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
+  <cols>
+    <col min="5" max="5" width="11.125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>44</v>
+      </c>
+      <c r="E1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+      <c r="G1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" t="s">
+        <v>49</v>
+      </c>
+      <c r="J1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>330</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>329</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>328</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>331</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>327</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="H2" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -14388,22 +14991,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4B00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4B00-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet87.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4C00-000000000000}">
+<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB2"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X2" sqref="X2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:28">
       <c r="A1" t="s">
@@ -14579,22 +15182,22 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com" xr:uid="{00000000-0004-0000-4C00-000000000000}"/>
-    <hyperlink ref="A2" r:id="rId2" xr:uid="{00000000-0004-0000-4C00-000001000000}"/>
+    <hyperlink ref="V2" r:id="rId1" display="mailto:guestPrivy@mailinator.com"/>
+    <hyperlink ref="A2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet88.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4D00-000000000000}">
+<file path=xl/worksheets/sheet92.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:14">
       <c r="A1" t="s">
@@ -14640,7 +15243,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="20">
+    <row r="2" spans="1:14" ht="20.25">
       <c r="A2" s="20" t="s">
         <v>162</v>
       </c>
@@ -14686,21 +15289,21 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H2" r:id="rId1" display="mw2demo_johnsmith@mailinator.com" xr:uid="{00000000-0004-0000-4D00-000000000000}"/>
+    <hyperlink ref="H2" r:id="rId1" display="mw2demo_johnsmith@mailinator.com"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet89.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4E00-000000000000}">
+<file path=xl/worksheets/sheet93.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
@@ -14738,96 +15341,14 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{00000000-0004-0000-4E00-000000000000}"/>
+    <hyperlink ref="A2" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:J2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
-  <cols>
-    <col min="5" max="5" width="11.1640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10">
-      <c r="A1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" t="s">
-        <v>61</v>
-      </c>
-      <c r="C1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D1" t="s">
-        <v>44</v>
-      </c>
-      <c r="E1" t="s">
-        <v>65</v>
-      </c>
-      <c r="F1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" t="s">
-        <v>48</v>
-      </c>
-      <c r="I1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J1" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>330</v>
-      </c>
-      <c r="C2" s="21" t="s">
-        <v>329</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>331</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>327</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet90.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-4F00-000000000000}">
+<file path=xl/worksheets/sheet94.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet15"/>
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -14835,7 +15356,7 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
   </cols>
@@ -14882,15 +15403,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{00000000-0004-0000-4F00-000000000000}"/>
-    <hyperlink ref="D2" r:id="rId2" xr:uid="{00000000-0004-0000-4F00-000001000000}"/>
+    <hyperlink ref="C2" r:id="rId1"/>
+    <hyperlink ref="D2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet91.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-5000-000000000000}">
+<file path=xl/worksheets/sheet95.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet16"/>
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -14898,7 +15419,7 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
@@ -14932,4 +15453,137 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet96.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:S2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.75"/>
+  <sheetData>
+    <row r="1" spans="1:19">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C1" t="s">
+        <v>444</v>
+      </c>
+      <c r="D1" t="s">
+        <v>445</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K1" t="s">
+        <v>64</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>65</v>
+      </c>
+      <c r="N1" t="s">
+        <v>215</v>
+      </c>
+      <c r="O1" t="s">
+        <v>46</v>
+      </c>
+      <c r="P1" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>48</v>
+      </c>
+      <c r="R1" t="s">
+        <v>49</v>
+      </c>
+      <c r="S1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" ht="18">
+      <c r="A2" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="52" t="s">
+        <v>446</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>447</v>
+      </c>
+      <c r="E2" t="s">
+        <v>251</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="G2" t="s">
+        <v>334</v>
+      </c>
+      <c r="H2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="O2" s="11" t="s">
+        <v>164</v>
+      </c>
+      <c r="P2" s="53" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>